<commit_message>
static analysis of reaction dFBA networks: generate networkX graph of reaction networks; perform path bounds analysis on dFBA submodels
also:
1. create & use method to generate Species ids, 2. use method to deterministically dedupe lists, 3. create method that gets products of objective function reactions
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="1600" yWindow="1460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1367,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1428,7 +1428,7 @@
         <v>105</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
making  columns implicit in Excel output
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,32 +26,37 @@
     <sheet name="Database references" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -63,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="139">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -113,301 +118,301 @@
     <t xml:space="preserve">Test model for TestExecutableModel</t>
   </si>
   <si>
+    <t xml:space="preserve">Rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rank not used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">References</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomass reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submodel_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism_biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submodel_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracellular space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typical density of Mycoplasma pneumoniae cells in culture is 1E9 cells/mL [Ref-0002].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empirical formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molecular weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pseudo_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2O2Na3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3SO4C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4[c] / k_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_id_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_comp_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_id_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_comp_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_id_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_comp_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_id_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass_comp_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism biomass reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No comment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rank not used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">References</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomass reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objective function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">submodel_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism_biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">submodel_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extracellular space</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typical density of Mycoplasma pneumoniae cells in culture is 1E9 cells/mL [Ref-0002].</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empirical formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molecular weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pseudo_species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2O2Na3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H3SO4C9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Observables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c] / k_m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_comp_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_comp_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_comp_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_comp_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism biomass reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No comment</t>
   </si>
   <si>
     <t xml:space="preserve">Submodels</t>
@@ -769,7 +774,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -862,53 +867,53 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>2000</v>
@@ -917,13 +922,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>0.0003</v>
@@ -934,13 +939,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>0.0003</v>
@@ -951,13 +956,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>0.0003</v>
@@ -991,8 +996,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="12" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="12" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="12" width="9.31983805668016"/>
@@ -1008,91 +1013,91 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>105</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>108</v>
-      </c>
       <c r="C3" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>112</v>
-      </c>
       <c r="C5" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="15" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1119,8 +1124,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="12" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="12" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="12" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -1132,27 +1137,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1179,12 +1184,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="43.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="43.5991902834008"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="49.165991902834"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1196,13 +1201,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>116</v>
@@ -1211,7 +1216,7 @@
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1252,18 +1257,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1271,12 +1276,9 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1296,19 +1298,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1023" min="5" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1319,56 +1322,54 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:D1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1407,22 +1408,22 @@
         <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>137</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>138</v>
@@ -1444,13 +1445,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6032388663968"/>
   </cols>
@@ -1476,12 +1477,12 @@
         <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>18</v>
@@ -1489,15 +1490,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="0" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1516,24 +1509,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="3" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1023" min="9" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1544,7 +1537,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>21</v>
@@ -1556,56 +1549,48 @@
         <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1624,20 +1609,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="44.7773279352227"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1648,54 +1634,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>4.58E-017</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="n">
-        <v>4.58E-017</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>1E-012</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>1E-012</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E3"/>
+  <autoFilter ref="A1:D3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1712,23 +1690,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="3" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1739,7 +1718,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>41</v>
@@ -1754,166 +1733,146 @@
         <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="0"/>
+      <c r="D2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0"/>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="0"/>
+      <c r="D3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0"/>
-      <c r="E3" s="3" t="s">
-        <v>52</v>
+      <c r="E3" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="0"/>
+      <c r="D4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0"/>
-      <c r="E4" s="3" t="s">
-        <v>55</v>
+      <c r="E4" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0"/>
+      <c r="D5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0"/>
-      <c r="E5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="E5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="F5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0"/>
+      <c r="D6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0"/>
-      <c r="E6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="0" t="n">
+      <c r="E6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="F6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="2" t="n">
+      <c r="E7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="8" t="n">
+      <c r="F7" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>49</v>
+      <c r="G7" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J6"/>
+  <autoFilter ref="A1:I6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1941,29 +1900,29 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="3" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>0.000148</v>
@@ -1971,7 +1930,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>0.0002</v>
@@ -1979,7 +1938,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>0.0005</v>
@@ -1987,7 +1946,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0.0005</v>
@@ -1995,7 +1954,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>0.001</v>
@@ -2003,7 +1962,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>0.002</v>
@@ -2025,18 +1984,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2044,15 +2003,12 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2072,13 +2028,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
@@ -2091,12 +2047,9 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2118,16 +2071,16 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="45.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2139,39 +2092,39 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -2187,16 +2140,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -2208,16 +2161,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -2229,16 +2182,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
cleaning up Model.get_* and Submodel.get_* methods; linking all top-level classes directly to Model
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,6 +56,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -78,6 +79,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -100,6 +102,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
@@ -122,6 +125,7 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -144,6 +148,7 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -801,11 +806,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -932,7 +937,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="1" sqref="C3 B1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1027,14 +1032,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" activeCellId="1" sqref="C3 D12"/>
+      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1087,118 +1092,126 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="9" min="1" style="8" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="13.3400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="10.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="42.004048582996"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="6" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="8" t="n">
+      <c r="E2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="8" t="n">
+      <c r="G2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+    <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="8" t="n">
+      <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1222,105 +1235,112 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="C3 H3"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.2024291497976"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1347,7 +1367,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="1" sqref="C3 C2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1410,7 +1430,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="1" sqref="C3 B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1533,7 +1553,7 @@
   <dimension ref="1:4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="C3 F8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1620,7 +1640,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C3 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1664,7 +1684,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="C3 D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1747,7 +1767,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1808,7 +1828,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="1" sqref="C3 B1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1876,7 +1896,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="1" sqref="C3 A2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1949,7 +1969,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2033,7 +2053,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="C3 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2227,7 +2247,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="1" sqref="C3 A2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2363,7 +2383,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="1" sqref="C3 I30"/>
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2500,29 +2520,33 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C3 E1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2544,29 +2568,33 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C3 E1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename RateLaw.equation --> expression
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -57,6 +57,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -80,6 +81,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -103,6 +105,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
@@ -126,6 +129,7 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -149,6 +153,7 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -160,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="159">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -478,9 +483,6 @@
   </si>
   <si>
     <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equation</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_1-forward</t>
@@ -1082,9 +1084,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="41.5627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1148,9 +1150,9 @@
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="13.3400809716599"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="10.0283400809717"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="42.004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="42.3117408906883"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="4" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="6" width="8.78542510121457"/>
   </cols>
@@ -1280,19 +1282,19 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.2024291497976"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.8097165991903"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1313,7 +1315,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>77</v>
@@ -1327,102 +1329,102 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>98</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1476,16 +1478,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>120</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>121</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1528,10 +1530,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>123</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>124</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>75</v>
@@ -1545,13 +1547,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>126</v>
-      </c>
       <c r="C2" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" s="21" t="n">
         <v>-3</v>
@@ -1560,19 +1562,19 @@
         <v>69</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>129</v>
-      </c>
       <c r="C3" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" s="21" t="n">
         <v>-4</v>
@@ -1583,13 +1585,13 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>131</v>
-      </c>
       <c r="C4" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="21" t="n">
         <v>1</v>
@@ -1600,13 +1602,13 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>133</v>
-      </c>
       <c r="C5" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="21" t="n">
         <v>2</v>
@@ -1633,7 +1635,7 @@
   </sheetPr>
   <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1673,31 +1675,31 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
@@ -1705,11 +1707,11 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
@@ -1797,46 +1799,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>33</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>16</v>
@@ -1873,19 +1875,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>86</v>
@@ -1900,7 +1902,7 @@
         <v>104</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
making DatabaseReferences inline; shortening database_references attribute to db_refs
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,67 +25,68 @@
     <sheet name="Parameters" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Stop conditions" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="References" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="Database references" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -112,6 +113,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
@@ -138,6 +140,7 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -164,6 +167,7 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -175,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="154">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -225,6 +229,9 @@
     <t xml:space="preserve">Author email</t>
   </si>
   <si>
+    <t xml:space="preserve">Database references</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
@@ -634,21 +641,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference</t>
   </si>
 </sst>
 </file>
@@ -700,17 +692,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -774,7 +766,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -807,28 +799,16 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -861,6 +841,14 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -961,12 +949,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1050,7 +1038,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1058,6 +1046,11 @@
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1079,21 +1072,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1105,27 +1098,30 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1144,24 +1140,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="4" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="4" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="6" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="10" min="5" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="6" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1172,39 +1168,42 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>0</v>
@@ -1215,38 +1214,38 @@
       <c r="G2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>1</v>
@@ -1254,16 +1253,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>103</v>
+        <v>31</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>0</v>
@@ -1287,21 +1286,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="24.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1313,125 +1312,128 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1450,51 +1452,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="18" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="15" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>24</v>
+      <c r="E1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>121</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1513,115 +1518,121 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="18" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="15" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="D1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>24</v>
+      <c r="G1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="21" t="n">
+      <c r="B2" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="18" t="n">
         <v>-3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="20"/>
+        <v>70</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="21" t="n">
+      <c r="B3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="18" t="n">
         <v>-4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="21" t="n">
+      <c r="B4" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="18" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="21" t="n">
+      <c r="B5" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>72</v>
+      <c r="E5" s="15" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1640,20 +1651,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="4" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1664,49 +1675,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AMJ1" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="4" t="s">
         <v>136</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
@@ -1714,11 +1727,11 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
@@ -1742,18 +1755,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1761,13 +1774,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1786,19 +1802,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="8" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="19" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="20" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1806,49 +1821,52 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q1" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1864,80 +1882,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" activeCellId="0" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.78542510121457"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1950,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1958,28 +1913,33 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2005,14 +1965,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1020" min="1" style="4" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1023" min="1021" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1021" min="1" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="5" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2023,41 +1982,43 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AMH1" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="AMI1" s="5"/>
-      <c r="AMJ1" s="0"/>
+      <c r="AMJ1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2076,10 +2037,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2095,54 +2056,59 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>4.58E-017</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>38</v>
+      <c r="E2" s="7"/>
+      <c r="F2" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>1E-012</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>41</v>
+      <c r="E3" s="7"/>
+      <c r="F3" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E3"/>
+  <autoFilter ref="A1:F3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2159,180 +2125,191 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="8" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="4" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="6" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>24</v>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="0"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="8" t="n">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="11"/>
+      <c r="G2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="0"/>
-      <c r="D3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8" t="n">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="0"/>
-      <c r="D4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8" t="n">
+      <c r="G4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="0"/>
-      <c r="D5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" s="8" t="n">
+      <c r="G5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="0"/>
-      <c r="D6" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="11"/>
+      <c r="G6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="12" t="n">
+        <v>65</v>
+      </c>
+      <c r="E7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="G7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I6"/>
+  <autoFilter ref="A1:J6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2349,20 +2326,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2373,105 +2350,114 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>35</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>35</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>35</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>35</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>35</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>35</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2489,19 +2475,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="14" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="12" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="11" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="10" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2512,104 +2498,113 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="15" t="n">
+        <v>79</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="12" t="n">
         <v>0.000148</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="E2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="12" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="15" t="n">
-        <v>0.0002</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="15" t="n">
+        <v>82</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="12" t="n">
         <v>0.0005</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="E4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="15" t="n">
+        <v>83</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="12" t="n">
         <v>0.0005</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="E5" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="15" t="n">
+        <v>84</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="12" t="n">
         <v>0.001</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="E6" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="15" t="n">
+        <v>85</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="12" t="n">
         <v>0.002</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="E7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2627,17 +2622,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.78542510121457"/>
   </cols>
@@ -2650,13 +2645,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2675,17 +2673,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.78542510121457"/>
   </cols>
@@ -2698,13 +2696,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding data structure for evidence
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,71 +24,76 @@
     <sheet name="dFBA net components" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Parameters" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Stop conditions" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="References" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Evidence" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="References" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -117,6 +122,8 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
@@ -145,34 +152,38 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -184,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="160">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -267,6 +278,9 @@
     <t xml:space="preserve">Algorithm</t>
   </si>
   <si>
+    <t xml:space="preserve">Evidence</t>
+  </si>
+  <si>
     <t xml:space="preserve">submodel_1</t>
   </si>
   <si>
@@ -610,6 +624,21 @@
   </si>
   <si>
     <t xml:space="preserve">K_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genetic variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature (C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth media</t>
   </si>
   <si>
     <t xml:space="preserve">Title</t>
@@ -658,7 +687,7 @@
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -692,6 +721,13 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -756,7 +792,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -819,6 +855,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -924,7 +964,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topRight" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1042,21 +1082,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1068,30 +1108,33 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1110,14 +1153,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1125,9 +1168,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="43.8097165991903"/>
-    <col collapsed="false" hidden="false" max="10" min="5" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="6" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="44.4534412955466"/>
+    <col collapsed="false" hidden="false" max="11" min="5" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="6" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1138,42 +1181,45 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1184,38 +1230,38 @@
       <c r="G2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1223,16 +1269,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1256,21 +1302,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1282,128 +1328,131 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1422,20 +1471,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="12" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="12" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1446,30 +1495,33 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>122</v>
+        <v>28</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1488,20 +1540,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="12" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="9" min="1" style="12" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1512,97 +1564,103 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="14"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D5" s="15" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1621,20 +1679,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="9" min="1" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="4" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1645,51 +1703,54 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" s="5" t="s">
         <v>137</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
@@ -1697,11 +1758,11 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
@@ -1725,34 +1786,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>86</v>
+      <c r="C1" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1772,18 +1840,99 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1791,46 +1940,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>16</v>
@@ -1936,13 +2085,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1021" min="1" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1022" min="1" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="4" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1959,37 +2108,39 @@
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AMI1" s="4"/>
       <c r="AMJ1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="5" t="s">
         <v>30</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2008,10 +2159,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2027,59 +2182,64 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>4.58E-017</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="5" t="s">
-        <v>39</v>
+      <c r="F2" s="7"/>
+      <c r="G2" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>1E-012</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="F3" s="5" t="s">
-        <v>42</v>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F3"/>
+  <autoFilter ref="A1:G3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2096,17 +2256,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.78542510121457"/>
   </cols>
@@ -2119,40 +2279,43 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2161,21 +2324,22 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2</v>
@@ -2184,21 +2348,22 @@
         <v>-1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3</v>
@@ -2207,21 +2372,22 @@
         <v>-2</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>4</v>
@@ -2230,21 +2396,22 @@
         <v>-5</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>5</v>
@@ -2253,20 +2420,21 @@
         <v>-3</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>6</v>
@@ -2275,12 +2443,13 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J6"/>
+  <autoFilter ref="A1:K6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2297,20 +2466,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="4" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="4" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="4" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2321,107 +2490,110 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2440,10 +2612,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2451,8 +2627,8 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="4" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="4" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2463,113 +2639,122 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>0.000148</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>0.0002</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>0.0005</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>0.0005</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>0.001</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>0.002</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2587,14 +2772,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2603,22 +2788,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>86</v>
+      <c r="C1" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2638,14 +2826,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA10" activeCellId="0" sqref="AA10"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2654,22 +2842,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>86</v>
+      <c r="C1" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changing initial_volume --> mean_volume; adding units for mean_volume; disabling 2d concentration units
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,42 +28,43 @@
     <sheet name="References" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
@@ -94,6 +95,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -124,6 +126,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
@@ -154,6 +157,7 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -184,6 +188,7 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -195,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="162">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -305,7 +310,10 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Initial volume</t>
+    <t xml:space="preserve">Mean volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean volume units</t>
   </si>
   <si>
     <t xml:space="preserve">c</t>
@@ -315,6 +323,9 @@
   </si>
   <si>
     <t xml:space="preserve">physical_3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
   </si>
   <si>
     <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
@@ -1094,9 +1105,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1108,10 +1119,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
@@ -1128,13 +1139,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1168,7 +1179,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="44.4534412955466"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="44.7773279352227"/>
     <col collapsed="false" hidden="false" max="11" min="5" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="6" width="8.78542510121457"/>
   </cols>
@@ -1181,19 +1192,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
@@ -1210,16 +1221,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1234,16 +1245,16 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1252,16 +1263,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1269,16 +1280,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1316,7 +1327,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1328,19 +1339,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
@@ -1357,102 +1368,102 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1495,7 +1506,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
@@ -1512,16 +1523,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1564,13 +1575,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
@@ -1587,80 +1598,80 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="14" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D5" s="15" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1706,10 +1717,10 @@
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
@@ -1726,31 +1737,31 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
@@ -1758,11 +1769,11 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
@@ -1809,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
@@ -1842,7 +1853,7 @@
   </sheetPr>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1852,8 +1863,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1865,28 +1876,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>16</v>
@@ -1940,46 +1951,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>16</v>
@@ -2159,14 +2170,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2188,58 +2199,67 @@
         <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>4.58E-017</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="5" t="s">
-        <v>40</v>
+      <c r="G2" s="7"/>
+      <c r="H2" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>1E-012</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="F3" s="7"/>
-      <c r="G3" s="5" t="s">
-        <v>43</v>
+      <c r="G3" s="7"/>
+      <c r="H3" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G3"/>
+  <autoFilter ref="A1:H3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2279,16 +2299,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>35</v>
@@ -2308,14 +2328,14 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2324,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -2332,14 +2352,14 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2</v>
@@ -2348,7 +2368,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -2356,14 +2376,14 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3</v>
@@ -2372,7 +2392,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2380,14 +2400,14 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>4</v>
@@ -2396,7 +2416,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2404,14 +2424,14 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>5</v>
@@ -2420,7 +2440,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2428,13 +2448,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>6</v>
@@ -2443,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -2490,10 +2510,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
@@ -2510,90 +2530,90 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2639,13 +2659,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
@@ -2662,96 +2682,96 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>0.000148</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>0.0002</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>0.0005</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>0.0005</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>0.001</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>0.002</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -2795,7 +2815,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
@@ -2849,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
adding standard deviation to mean volume, mean concentration
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -28,43 +28,46 @@
     <sheet name="References" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
@@ -96,6 +99,9 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -127,6 +133,9 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
@@ -158,6 +167,9 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -189,6 +201,9 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -200,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="165">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -310,10 +325,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean volume units</t>
+    <t xml:space="preserve">Volume mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume units</t>
   </si>
   <si>
     <t xml:space="preserve">c</t>
@@ -442,175 +460,181 @@
     <t xml:space="preserve">Species</t>
   </si>
   <si>
+    <t xml:space="preserve">Mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_1[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_2[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_4[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_5[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-obj-submodel_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_1-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s^-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_2-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_2 * specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4[c] / k_m_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3-backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_4-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism_net_rxn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism net reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_1[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net component 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net component 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_3[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net component 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_4[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net component 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc-specie_1[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc-specie_2[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc-specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc-specie_4[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc-specie_5[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conc-specie_6[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-obj-submodel_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_1-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s^-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_2-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat_2 * specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c] / k_m_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3-backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_4-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism_net_rxn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism net reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coefficient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_1[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net component 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net component 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_3[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net component 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_4[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net component 4</t>
   </si>
   <si>
     <t xml:space="preserve">fractionDryWeight</t>
@@ -1105,9 +1129,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1119,10 +1143,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
@@ -1139,13 +1163,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1203,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="44.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="45.9554655870445"/>
     <col collapsed="false" hidden="false" max="11" min="5" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="6" width="8.78542510121457"/>
   </cols>
@@ -1192,19 +1216,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
@@ -1221,16 +1245,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1245,16 +1269,16 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1263,16 +1287,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1280,16 +1304,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1327,7 +1351,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1339,19 +1363,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
@@ -1368,102 +1392,102 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1506,7 +1530,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
@@ -1523,16 +1547,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1575,13 +1599,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
@@ -1598,80 +1622,80 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D5" s="15" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1717,10 +1741,10 @@
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
@@ -1737,31 +1761,31 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
@@ -1769,11 +1793,11 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
@@ -1820,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
@@ -1863,8 +1887,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1876,28 +1900,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>16</v>
@@ -1951,46 +1975,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>16</v>
@@ -2170,14 +2194,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2202,64 +2226,73 @@
         <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>4.58E-017</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="7"/>
+      <c r="E2" s="7" t="n">
+        <v>4.58E-018</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="G2" s="7"/>
-      <c r="H2" s="5" t="s">
-        <v>42</v>
+      <c r="H2" s="7"/>
+      <c r="I2" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>1E-012</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="7"/>
+      <c r="E3" s="7" t="n">
+        <v>1E-013</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="G3" s="7"/>
-      <c r="H3" s="5" t="s">
-        <v>45</v>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H3"/>
+  <autoFilter ref="A1:I3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2299,16 +2332,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>35</v>
@@ -2328,14 +2361,14 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2344,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -2352,14 +2385,14 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2</v>
@@ -2368,7 +2401,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -2376,14 +2409,14 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3</v>
@@ -2392,7 +2425,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2400,14 +2433,14 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>4</v>
@@ -2416,7 +2449,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2424,14 +2457,14 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>5</v>
@@ -2440,7 +2473,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2448,13 +2481,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>6</v>
@@ -2463,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -2510,10 +2543,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
@@ -2530,90 +2563,90 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2632,14 +2665,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2647,8 +2680,8 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="4" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="5" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="4" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2659,122 +2692,143 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>0.000148</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="9"/>
+      <c r="E2" s="9" t="n">
+        <v>0.0121655250605964</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>0.0002</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="9"/>
+      <c r="E3" s="9" t="n">
+        <v>0.014142135623731</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>0.0005</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="9"/>
+      <c r="E4" s="9" t="n">
+        <v>0.0223606797749979</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>0.0005</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="9"/>
+      <c r="E5" s="9" t="n">
+        <v>0.0223606797749979</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>0.001</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="9"/>
+      <c r="E6" s="9" t="n">
+        <v>0.0316227766016838</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>0.002</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="9"/>
+      <c r="E7" s="9" t="n">
+        <v>0.0447213595499958</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2815,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
@@ -2869,7 +2923,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
adding more units attributes, documentation
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -72,6 +72,9 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
@@ -110,6 +113,9 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -148,6 +154,9 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
@@ -186,6 +195,9 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -224,6 +236,9 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -235,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="172">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -519,6 +534,9 @@
     <t xml:space="preserve">Expression</t>
   </si>
   <si>
+    <t xml:space="preserve">Concentration units</t>
+  </si>
+  <si>
     <t xml:space="preserve">Submodel</t>
   </si>
   <si>
@@ -528,6 +546,9 @@
     <t xml:space="preserve">reaction_1</t>
   </si>
   <si>
+    <t xml:space="preserve">gsCellCycle gCell^-1 s^-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Participants</t>
   </si>
   <si>
@@ -549,7 +570,7 @@
     <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
   </si>
   <si>
-    <t xml:space="preserve">mol g^-1 s^-1</t>
+    <t xml:space="preserve">mol reaction gCell^-1 s^-1</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_2</t>
@@ -597,7 +618,10 @@
     <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
   </si>
   <si>
-    <t xml:space="preserve">s^-1</t>
+    <t xml:space="preserve">reaction cell^-1 s^-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">molecule cell^-1</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_2-forward</t>
@@ -645,7 +669,7 @@
     <t xml:space="preserve">dFBA net component 1</t>
   </si>
   <si>
-    <t xml:space="preserve">M s^-1</t>
+    <t xml:space="preserve">mol gsCellCycle^-1</t>
   </si>
   <si>
     <t xml:space="preserve">test</t>
@@ -859,7 +883,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -922,6 +946,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1160,21 +1188,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.5951417004049"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1186,33 +1214,39 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1234,11 +1268,11 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1246,7 +1280,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="47.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="48.6315789473684"/>
     <col collapsed="false" hidden="false" max="12" min="5" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="6" width="8.78542510121457"/>
   </cols>
@@ -1259,22 +1293,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -1291,16 +1325,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1312,22 +1346,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1336,16 +1370,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1353,16 +1387,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1386,21 +1420,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.62753036437247"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1412,10 +1447,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>37</v>
@@ -1427,116 +1462,134 @@
         <v>85</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>120</v>
+      <c r="H3" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1558,9 +1611,9 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
@@ -1579,7 +1632,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>18</v>
@@ -1596,16 +1649,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1631,7 +1684,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1650,13 +1703,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>82</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>85</v>
@@ -1676,13 +1729,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>76</v>
@@ -1690,25 +1743,25 @@
       <c r="E2" s="15" t="n">
         <v>-3</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>136</v>
+      <c r="F2" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>77</v>
@@ -1716,21 +1769,21 @@
       <c r="E3" s="15" t="n">
         <v>-4</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>136</v>
+      <c r="F3" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>78</v>
@@ -1738,21 +1791,21 @@
       <c r="E4" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>136</v>
+      <c r="F4" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>79</v>
@@ -1760,8 +1813,8 @@
       <c r="E5" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>136</v>
+      <c r="F5" s="16" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1807,7 +1860,7 @@
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>85</v>
@@ -1827,31 +1880,31 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
@@ -1859,11 +1912,11 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
@@ -1887,19 +1940,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1023" min="1" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1916,15 +1970,18 @@
         <v>85</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1961,46 +2018,46 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="G1" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="H1" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2043,46 +2100,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2968,14 +3025,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2994,15 +3051,21 @@
         <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removing unused fixture; adding standard error to Parameter; making Parameter units required; adding density to Compartment
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,53 +28,54 @@
     <sheet name="References" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$I$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
@@ -116,6 +117,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -157,47 +159,49 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -239,6 +243,7 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -250,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="178">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -375,6 +380,15 @@
     <t xml:space="preserve">Volume units</t>
   </si>
   <si>
+    <t xml:space="preserve">Density mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density units</t>
+  </si>
+  <si>
     <t xml:space="preserve">c</t>
   </si>
   <si>
@@ -384,7 +398,10 @@
     <t xml:space="preserve">physical_3d</t>
   </si>
   <si>
-    <t xml:space="preserve">L</t>
+    <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g ml^-1</t>
   </si>
   <si>
     <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
@@ -693,6 +710,9 @@
     <t xml:space="preserve">dFBA net component 4</t>
   </si>
   <si>
+    <t xml:space="preserve">Standard error</t>
+  </si>
+  <si>
     <t xml:space="preserve">fractionDryWeight</t>
   </si>
   <si>
@@ -709,6 +729,9 @@
   </si>
   <si>
     <t xml:space="preserve">k_cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction molecule^-1 s^-1</t>
   </si>
   <si>
     <t xml:space="preserve">k_m_3</t>
@@ -1190,17 +1213,17 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="I41" activeCellId="0" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
@@ -1214,13 +1237,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -1237,16 +1260,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1295,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1280,7 +1303,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="48.6315789473684"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="49.0607287449393"/>
     <col collapsed="false" hidden="false" max="12" min="5" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="6" width="8.78542510121457"/>
   </cols>
@@ -1293,22 +1316,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -1325,16 +1348,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1346,22 +1369,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="L2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1370,16 +1393,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1387,16 +1410,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1427,15 +1450,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="H34" activeCellId="0" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.62753036437247"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.60728744939271"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1447,22 +1470,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -1479,117 +1502,117 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1611,11 +1634,11 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1632,7 +1655,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>18</v>
@@ -1649,16 +1672,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1684,13 +1707,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="12" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="10" min="7" style="12" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="3" width="8.78542510121457"/>
   </cols>
@@ -1703,16 +1726,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -1729,92 +1752,92 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E5" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1833,20 +1856,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="O30" activeCellId="0" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="9" min="1" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="4" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1860,70 +1885,82 @@
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>150</v>
+      <c r="E2" s="0"/>
+      <c r="F2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
       </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
       </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:F1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1947,13 +1984,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="N32" activeCellId="0" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1023" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="4" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1964,13 +2001,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2008,7 +2045,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="Q36" activeCellId="0" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -2025,28 +2062,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>37</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>18</v>
@@ -2084,7 +2121,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="S36" activeCellId="0" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -2100,46 +2137,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2319,14 +2356,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2354,27 +2391,36 @@
         <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>4.58E-017</v>
@@ -2383,23 +2429,30 @@
         <v>4.58E-018</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>1E-012</v>
@@ -2408,16 +2461,23 @@
         <v>1E-013</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.99318</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I3"/>
+  <autoFilter ref="A1:L3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2457,16 +2517,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>37</v>
@@ -2486,14 +2546,14 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2502,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -2510,14 +2570,14 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2</v>
@@ -2526,7 +2586,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -2534,14 +2594,14 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3</v>
@@ -2550,7 +2610,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2558,14 +2618,14 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>4</v>
@@ -2574,7 +2634,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2582,14 +2642,14 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>5</v>
@@ -2598,7 +2658,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2606,13 +2666,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>6</v>
@@ -2621,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -2668,10 +2728,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2688,90 +2748,90 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2817,16 +2877,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2843,10 +2903,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>0.000148</v>
@@ -2855,17 +2915,17 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>0.0002</v>
@@ -2874,17 +2934,17 @@
         <v>0.014142135623731</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>0.0005</v>
@@ -2893,17 +2953,17 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>0.0005</v>
@@ -2912,17 +2972,17 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>0.001</v>
@@ -2931,17 +2991,17 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>0.002</v>
@@ -2950,7 +3010,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -2978,7 +3038,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="I41" activeCellId="0" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2994,7 +3054,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>18</v>
@@ -3032,7 +3092,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="J40" activeCellId="0" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3048,13 +3108,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
introduced compiled expression attribute which is faster and more accurate; removing concentration_units attribute and replacing with exposure of compartment volumes in functions, rate laws, and stop conditions
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="177">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -551,9 +551,6 @@
     <t xml:space="preserve">Expression</t>
   </si>
   <si>
-    <t xml:space="preserve">Concentration units</t>
-  </si>
-  <si>
     <t xml:space="preserve">Submodel</t>
   </si>
   <si>
@@ -638,106 +635,106 @@
     <t xml:space="preserve">reaction cell^-1 s^-1</t>
   </si>
   <si>
+    <t xml:space="preserve">reaction_2-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_2 * specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4[c] / k_m_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3-backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_4-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism_net_rxn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism net reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_1[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net component 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mol gsCellCycle^-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net component 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_3[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net component 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_4[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dFBA net component 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionDryWeight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of cell mass which is non water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimensionless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Ref-0006]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction molecule^-1 s^-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_m_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K_m</t>
+  </si>
+  <si>
     <t xml:space="preserve">molecule cell^-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_2-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat_2 * specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c] / k_m_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3-backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_4-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism_net_rxn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism net reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_1[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net component 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol gsCellCycle^-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net component 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_3[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net component 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-specie_4[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dFBA net component 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fractionDryWeight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fraction of cell mass which is non water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dimensionless</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Ref-0006]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction molecule^-1 s^-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_m_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K_m</t>
   </si>
   <si>
     <t xml:space="preserve">Taxon</t>
@@ -1237,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>97</v>
@@ -1260,16 +1257,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1316,22 +1313,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -1348,16 +1345,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1369,22 +1366,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1393,16 +1390,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1410,16 +1407,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1443,14 +1440,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H34" activeCellId="0" sqref="H34"/>
+      <selection pane="bottomRight" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1459,7 +1456,8 @@
     <col collapsed="false" hidden="false" max="4" min="2" style="1" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.60728744939271"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1023" min="7" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1470,10 +1468,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>37</v>
@@ -1485,134 +1483,116 @@
         <v>89</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>81</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1655,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>18</v>
@@ -1672,16 +1652,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1726,13 +1706,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>86</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>89</v>
@@ -1752,13 +1732,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>80</v>
@@ -1767,24 +1747,24 @@
         <v>-3</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>81</v>
@@ -1793,20 +1773,20 @@
         <v>-4</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>82</v>
@@ -1815,20 +1795,20 @@
         <v>1</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>83</v>
@@ -1837,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1885,10 +1865,10 @@
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>89</v>
@@ -1908,55 +1888,55 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="0"/>
       <c r="F2" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1977,20 +1957,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N32" activeCellId="0" sqref="N32"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1022" min="1" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2007,18 +1988,15 @@
         <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2062,7 +2040,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>89</v>
@@ -2071,19 +2049,19 @@
         <v>37</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>18</v>
@@ -2137,46 +2115,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2358,7 +2336,7 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -3031,14 +3009,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I41" activeCellId="0" sqref="I41"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3057,15 +3035,18 @@
         <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3085,19 +3066,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J40" activeCellId="0" sqref="J40"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1023" min="1" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3114,18 +3096,15 @@
         <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- adding units to species, observable, dFBA net reaction - fixing DfbaObjectiveCoefficientUnit - adding unit validation for functions, rate laws, stop conditions - adding compiled expression to ParsedExpression for evaluation
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="182">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -491,9 +491,15 @@
     <t xml:space="preserve">Compartment</t>
   </si>
   <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
     <t xml:space="preserve">specie_1[e]</t>
   </si>
   <si>
+    <t xml:space="preserve">molecule cell^-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">specie_2[e]</t>
   </si>
   <si>
@@ -524,9 +530,6 @@
     <t xml:space="preserve">Standard deviation</t>
   </si>
   <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
     <t xml:space="preserve">conc-specie_1[e]</t>
   </si>
   <si>
@@ -629,7 +632,7 @@
     <t xml:space="preserve">other</t>
   </si>
   <si>
-    <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
+    <t xml:space="preserve">k_cat_1 * max( specie_1[e], specie_2[e] )</t>
   </si>
   <si>
     <t xml:space="preserve">reaction cell^-1 s^-1</t>
@@ -644,7 +647,7 @@
     <t xml:space="preserve">reaction_3-forward</t>
   </si>
   <si>
-    <t xml:space="preserve">specie_4[c] / k_m_3</t>
+    <t xml:space="preserve">k_cat_3 * specie_4[c] / k_m_3</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_3-backward</t>
@@ -653,12 +656,15 @@
     <t xml:space="preserve">backward</t>
   </si>
   <si>
-    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
+    <t xml:space="preserve">k_cat_4 * (specie_5[c] + specie_6[c])</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_4-forward</t>
   </si>
   <si>
+    <t xml:space="preserve">k_cat_5 * specie_2[c]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Metabolism_net_rxn</t>
   </si>
   <si>
@@ -734,7 +740,16 @@
     <t xml:space="preserve">K_m</t>
   </si>
   <si>
-    <t xml:space="preserve">molecule cell^-1</t>
+    <t xml:space="preserve">k_cat_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_5</t>
   </si>
   <si>
     <t xml:space="preserve">Taxon</t>
@@ -903,7 +918,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -970,6 +985,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1234,13 +1253,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -1257,16 +1276,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1313,22 +1332,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -1345,16 +1364,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1366,22 +1385,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1390,16 +1409,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1407,16 +1426,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1442,12 +1461,12 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1468,19 +1487,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -1497,102 +1516,114 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1611,20 +1642,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="12" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="12" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1635,33 +1666,39 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>136</v>
+      <c r="D2" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1706,16 +1743,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -1732,92 +1769,92 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E5" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1836,25 +1873,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O30" activeCellId="0" sqref="O30"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="5" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="5" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="10" min="7" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="6" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1865,13 +1902,13 @@
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -1888,55 +1925,111 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="E2" s="0"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>155</v>
+      <c r="A3" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>158</v>
+      <c r="A4" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>159</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1982,10 +2075,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2033,46 +2126,46 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="K1" s="17" t="s">
+      <c r="F1" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="18" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2115,46 +2208,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2682,20 +2775,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="4" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="9" min="1" style="4" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="4" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2712,21 +2805,24 @@
         <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>57</v>
@@ -2734,10 +2830,13 @@
       <c r="D2" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>61</v>
@@ -2745,10 +2844,13 @@
       <c r="D3" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>57</v>
@@ -2756,10 +2858,13 @@
       <c r="D4" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>61</v>
@@ -2767,10 +2872,13 @@
       <c r="D5" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>64</v>
@@ -2778,10 +2886,13 @@
       <c r="D6" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>67</v>
@@ -2789,10 +2900,13 @@
       <c r="D7" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>70</v>
@@ -2800,16 +2914,22 @@
       <c r="D8" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>44</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2855,16 +2975,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2881,10 +3001,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>0.000148</v>
@@ -2893,17 +3013,17 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>0.0002</v>
@@ -2912,17 +3032,17 @@
         <v>0.014142135623731</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>0.0005</v>
@@ -2931,17 +3051,17 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>0.0005</v>
@@ -2950,17 +3070,17 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>0.001</v>
@@ -2969,17 +3089,17 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>0.002</v>
@@ -2988,7 +3108,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -3011,12 +3131,12 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3032,10 +3152,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -3090,10 +3210,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
normalizing units of dFBA within WC models
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="182">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -310,6 +310,12 @@
     <t xml:space="preserve">Author email</t>
   </si>
   <si>
+    <t xml:space="preserve">Cell mass units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
     <t xml:space="preserve">Time units</t>
   </si>
   <si>
@@ -568,7 +574,7 @@
     <t xml:space="preserve">reaction_1</t>
   </si>
   <si>
-    <t xml:space="preserve">gsCellCycle gCell^-1 s^-1</t>
+    <t xml:space="preserve">dimensionless</t>
   </si>
   <si>
     <t xml:space="preserve">Participants</t>
@@ -592,7 +598,7 @@
     <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
   </si>
   <si>
-    <t xml:space="preserve">mol reaction gCell^-1 s^-1</t>
+    <t xml:space="preserve">M s^-1</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_2</t>
@@ -640,7 +646,7 @@
     <t xml:space="preserve">k_cat_1 * max( specie_1[e], specie_2[e] )</t>
   </si>
   <si>
-    <t xml:space="preserve">reaction s^-1</t>
+    <t xml:space="preserve">s^-1</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_2-forward</t>
@@ -691,9 +697,6 @@
     <t xml:space="preserve">dFBA net component 1</t>
   </si>
   <si>
-    <t xml:space="preserve">mol gsCellCycle^-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">test</t>
   </si>
   <si>
@@ -724,9 +727,6 @@
     <t xml:space="preserve">Fraction of cell mass which is non water</t>
   </si>
   <si>
-    <t xml:space="preserve">dimensionless</t>
-  </si>
-  <si>
     <t xml:space="preserve">[Ref-0006]</t>
   </si>
   <si>
@@ -736,7 +736,7 @@
     <t xml:space="preserve">k_cat</t>
   </si>
   <si>
-    <t xml:space="preserve">reaction molecule^-1 s^-1</t>
+    <t xml:space="preserve">molecule^-1 s^-1</t>
   </si>
   <si>
     <t xml:space="preserve">k_m_3</t>
@@ -1098,12 +1098,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1189,7 +1189,7 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="0" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1197,20 +1197,28 @@
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1247,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I41" activeCellId="0" sqref="I41"/>
+      <selection pane="bottomRight" activeCell="E3" activeCellId="1" sqref="A11:B11 E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1258,39 +1266,39 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1316,7 +1324,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H40" activeCellId="0" sqref="H40"/>
+      <selection pane="bottomRight" activeCell="H3" activeCellId="1" sqref="A11:B11 H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1337,48 +1345,48 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1390,22 +1398,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1414,16 +1422,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1431,16 +1439,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1466,12 +1474,12 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N12" activeCellId="0" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="J26" activeCellId="1" sqref="A11:B11 J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1492,51 +1500,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
@@ -1544,22 +1552,22 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
@@ -1567,22 +1575,22 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I4" s="0"/>
       <c r="J4" s="0"/>
@@ -1590,22 +1598,22 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I5" s="0"/>
       <c r="J5" s="0"/>
@@ -1613,22 +1621,22 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1654,7 +1662,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L24" activeCellId="0" sqref="L24"/>
+      <selection pane="bottomRight" activeCell="D3" activeCellId="1" sqref="A11:B11 D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1671,39 +1679,39 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1729,7 +1737,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M29" activeCellId="0" sqref="M29"/>
+      <selection pane="bottomRight" activeCell="L17" activeCellId="1" sqref="A11:B11 L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1748,118 +1756,118 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E5" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1885,7 +1893,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="K34" activeCellId="1" sqref="A11:B11 K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1904,46 +1912,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="5" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>155</v>
@@ -1978,7 +1986,7 @@
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2005,8 +2013,8 @@
       <c r="D6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>126</v>
+      <c r="F6" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2062,7 +2070,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="1" sqref="A11:B11 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2080,22 +2088,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2121,7 +2129,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q36" activeCellId="0" sqref="Q36"/>
+      <selection pane="bottomRight" activeCell="Q36" activeCellId="1" sqref="A11:B11 Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -2138,13 +2146,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>165</v>
@@ -2162,16 +2170,16 @@
         <v>169</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="18" t="s">
         <v>29</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2197,7 +2205,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S36" activeCellId="0" sqref="S36"/>
+      <selection pane="bottomRight" activeCell="S36" activeCellId="1" sqref="A11:B11 S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -2225,7 +2233,7 @@
         <v>172</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>173</v>
@@ -2255,10 +2263,10 @@
         <v>181</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2284,7 +2292,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topRight" activeCell="C9" activeCellId="1" sqref="A11:B11 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2297,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2305,34 +2313,34 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2358,7 +2366,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="A11:B11 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2375,45 +2383,45 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="AMJ1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2439,7 +2447,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M28" activeCellId="0" sqref="M28"/>
+      <selection pane="bottomRight" activeCell="M28" activeCellId="1" sqref="A11:B11 M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2455,48 +2463,48 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>4.58E-017</v>
@@ -2505,30 +2513,30 @@
         <v>4.58E-018</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>1.09</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>1E-012</v>
@@ -2537,19 +2545,19 @@
         <v>1E-013</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.99318</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2577,7 +2585,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="1" sqref="A11:B11 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2593,43 +2601,43 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2638,7 +2646,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -2646,14 +2654,14 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2</v>
@@ -2662,7 +2670,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -2670,14 +2678,14 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3</v>
@@ -2686,7 +2694,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2694,14 +2702,14 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>4</v>
@@ -2710,7 +2718,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2718,14 +2726,14 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>5</v>
@@ -2734,7 +2742,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2742,13 +2750,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>6</v>
@@ -2757,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -2787,7 +2795,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G25" activeCellId="0" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="G25" activeCellId="1" sqref="A11:B11 G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2804,137 +2812,137 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2960,7 +2968,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="1" sqref="A11:B11 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2980,36 +2988,36 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>0.000148</v>
@@ -3018,17 +3026,17 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>0.0002</v>
@@ -3037,17 +3045,17 @@
         <v>0.014142135623731</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>0.0005</v>
@@ -3056,17 +3064,17 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>0.0005</v>
@@ -3075,17 +3083,17 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>0.001</v>
@@ -3094,17 +3102,17 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>0.002</v>
@@ -3113,7 +3121,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -3141,7 +3149,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L26" activeCellId="0" sqref="L26"/>
+      <selection pane="bottomRight" activeCell="L26" activeCellId="1" sqref="A11:B11 L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3157,22 +3165,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3194,11 +3202,11 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="P36" activeCellId="1" sqref="A11:B11 P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3215,22 +3223,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replacing Model.cell_mass_units with DfbaNetReaction.cell_size_units
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,9 +17,9 @@
     <sheet name="Concentrations" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Observables" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="dFBA objectives" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Reactions" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Rate laws" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="dFBA objectives" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="dFBA net reactions" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="dFBA net components" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Parameters" sheetId="15" state="visible" r:id="rId16"/>
@@ -30,7 +30,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$L$3</definedName>
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
@@ -120,49 +120,49 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="181">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -310,12 +310,6 @@
     <t xml:space="preserve">Author email</t>
   </si>
   <si>
-    <t xml:space="preserve">Cell mass units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g</t>
-  </si>
-  <si>
     <t xml:space="preserve">Time units</t>
   </si>
   <si>
@@ -568,112 +562,115 @@
     <t xml:space="preserve">Submodel</t>
   </si>
   <si>
+    <t xml:space="preserve">Participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M s^-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_1-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_1 * max( specie_1[e], specie_2[e] )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s^-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_2-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_2 * specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_3 * specie_4[c] / k_m_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3-backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_4 * (specie_5[c] + specie_6[c])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_4-forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_5 * specie_2[c]</t>
+  </si>
+  <si>
     <t xml:space="preserve">dfba-obj-submodel_1</t>
   </si>
   <si>
-    <t xml:space="preserve">reaction_1</t>
-  </si>
-  <si>
     <t xml:space="preserve">dimensionless</t>
   </si>
   <si>
-    <t xml:space="preserve">Participants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M s^-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_1-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat_1 * max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s^-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_2-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat_2 * specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat_3 * specie_4[c] / k_m_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3-backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat_4 * (specie_5[c] + specie_6[c])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_4-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat_5 * specie_2[c]</t>
+    <t xml:space="preserve">Cell size units</t>
   </si>
   <si>
     <t xml:space="preserve">Metabolism_net_rxn</t>
@@ -1098,12 +1095,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11:B11"/>
+      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1189,7 +1186,7 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1197,30 +1194,23 @@
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="https://github.com/org/repo"/>
@@ -1240,83 +1230,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" activeCellId="1" sqref="A11:B11 E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1324,7 +1237,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" activeCellId="1" sqref="A11:B11 H3"/>
+      <selection pane="bottomRight" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1345,48 +1258,48 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1398,22 +1311,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1422,16 +1335,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1439,16 +1352,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1467,7 +1380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1479,7 +1392,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J26" activeCellId="1" sqref="A11:B11 J26"/>
+      <selection pane="bottomRight" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1500,51 +1413,51 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
@@ -1552,22 +1465,22 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
@@ -1575,22 +1488,22 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I4" s="0"/>
       <c r="J4" s="0"/>
@@ -1598,22 +1511,22 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I5" s="0"/>
       <c r="J5" s="0"/>
@@ -1621,22 +1534,22 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1650,25 +1563,102 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I18" activeCellId="0" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" activeCellId="1" sqref="A11:B11 D3"/>
+      <selection pane="bottomRight" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="12" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="9" min="1" style="12" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1679,39 +1669,45 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>78</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1737,7 +1733,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L17" activeCellId="1" sqref="A11:B11 L17"/>
+      <selection pane="bottomRight" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1756,118 +1752,118 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="F1" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>144</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>147</v>
-      </c>
       <c r="C3" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>149</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>151</v>
-      </c>
       <c r="C5" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1893,7 +1889,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K34" activeCellId="1" sqref="A11:B11 K34"/>
+      <selection pane="bottomRight" activeCell="K34" activeCellId="0" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1912,137 +1908,137 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>154</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="5" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2070,7 +2066,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" activeCellId="1" sqref="A11:B11 E2"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2088,22 +2084,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2129,7 +2125,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q36" activeCellId="1" sqref="A11:B11 Q36"/>
+      <selection pane="bottomRight" activeCell="Q36" activeCellId="0" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -2146,40 +2142,40 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="J1" s="18" t="s">
-        <v>169</v>
-      </c>
       <c r="K1" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2205,7 +2201,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S36" activeCellId="1" sqref="A11:B11 S36"/>
+      <selection pane="bottomRight" activeCell="S36" activeCellId="0" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -2221,52 +2217,52 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2288,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C9" activeCellId="1" sqref="A11:B11 C9"/>
+      <selection pane="topRight" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2305,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2313,34 +2309,34 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2366,7 +2362,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="A11:B11 E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2383,45 +2379,45 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AMJ1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2447,7 +2443,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M28" activeCellId="1" sqref="A11:B11 M28"/>
+      <selection pane="bottomRight" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2463,48 +2459,48 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>4.58E-017</v>
@@ -2513,30 +2509,30 @@
         <v>4.58E-018</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>1.09</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>1E-012</v>
@@ -2545,19 +2541,19 @@
         <v>1E-013</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.99318</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2585,7 +2581,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="1" sqref="A11:B11 I1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2601,43 +2597,43 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2646,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -2654,14 +2650,14 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2</v>
@@ -2670,7 +2666,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -2678,14 +2674,14 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>3</v>
@@ -2694,7 +2690,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2702,14 +2698,14 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>4</v>
@@ -2718,7 +2714,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2726,14 +2722,14 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>5</v>
@@ -2742,7 +2738,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2750,13 +2746,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>6</v>
@@ -2765,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -2795,7 +2791,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G25" activeCellId="1" sqref="A11:B11 G25"/>
+      <selection pane="bottomRight" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2812,137 +2808,137 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2968,7 +2964,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="1" sqref="A11:B11 D2"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2988,36 +2984,36 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D2" s="9" t="n">
         <v>0.000148</v>
@@ -3026,17 +3022,17 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>0.0002</v>
@@ -3045,17 +3041,17 @@
         <v>0.014142135623731</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>0.0005</v>
@@ -3064,17 +3060,17 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>0.0005</v>
@@ -3083,17 +3079,17 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" s="9" t="n">
         <v>0.001</v>
@@ -3102,17 +3098,17 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="9" t="n">
         <v>0.002</v>
@@ -3121,7 +3117,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -3149,7 +3145,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L26" activeCellId="1" sqref="A11:B11 L26"/>
+      <selection pane="bottomRight" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3165,22 +3161,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3206,7 +3202,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
-      <selection pane="bottomRight" activeCell="P36" activeCellId="1" sqref="A11:B11 P36"/>
+      <selection pane="bottomRight" activeCell="P36" activeCellId="0" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3223,22 +3219,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clarifying semantics of initial concentrations
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
     <sheet name="Compartments" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Species types" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Species" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Concentrations" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Distributions of initial concentrations of species" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Observables" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="183">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -529,6 +529,9 @@
     <t xml:space="preserve">Species</t>
   </si>
   <si>
+    <t xml:space="preserve">Distribution</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mean</t>
   </si>
   <si>
@@ -536,6 +539,9 @@
   </si>
   <si>
     <t xml:space="preserve">conc-specie_1[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
   </si>
   <si>
     <t xml:space="preserve">M</t>
@@ -1258,22 +1264,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -1290,16 +1296,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>0</v>
@@ -1311,22 +1317,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1335,16 +1341,16 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>1</v>
@@ -1352,16 +1358,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>0</v>
@@ -1413,16 +1419,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>78</v>
@@ -1442,22 +1448,22 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
@@ -1465,22 +1471,22 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
@@ -1488,22 +1494,22 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I4" s="0"/>
       <c r="J4" s="0"/>
@@ -1511,22 +1517,22 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I5" s="0"/>
       <c r="J5" s="0"/>
@@ -1534,22 +1540,22 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1570,7 +1576,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1594,10 +1600,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>78</v>
@@ -1617,16 +1623,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1669,13 +1675,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>78</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -1692,22 +1698,22 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>47</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1752,13 +1758,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>88</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>78</v>
@@ -1778,13 +1784,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>82</v>
@@ -1793,24 +1799,24 @@
         <v>-3</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>83</v>
@@ -1819,20 +1825,20 @@
         <v>-4</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>84</v>
@@ -1841,20 +1847,20 @@
         <v>1</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>85</v>
@@ -1863,7 +1869,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1911,10 +1917,10 @@
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>78</v>
@@ -1934,48 +1940,48 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>0.3</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0.001</v>
@@ -1987,58 +1993,58 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2084,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>78</v>
@@ -2142,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>78</v>
@@ -2151,19 +2157,19 @@
         <v>37</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>18</v>
@@ -2217,46 +2223,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2957,23 +2963,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="4" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="5" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="10" min="5" style="5" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="4" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="5" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="5" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="4" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2993,134 +2999,155 @@
         <v>90</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="9" t="n">
         <v>0.000148</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="F2" s="9" t="n">
         <v>0.0121655250605964</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="9" t="n">
         <v>0.0002</v>
       </c>
-      <c r="E3" s="9" t="n">
+      <c r="F3" s="9" t="n">
         <v>0.014142135623731</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="9" t="n">
         <v>0.0005</v>
       </c>
-      <c r="E4" s="9" t="n">
+      <c r="F4" s="9" t="n">
         <v>0.0223606797749979</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="9" t="n">
         <v>0.0005</v>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="F5" s="9" t="n">
         <v>0.0223606797749979</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="9" t="n">
         <v>0.001</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="F6" s="9" t="n">
         <v>0.0316227766016838</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="9" t="n">
         <v>0.002</v>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="F7" s="9" t="n">
         <v>0.0447213595499958</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3161,7 +3188,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>78</v>
@@ -3219,7 +3246,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
adding back initial volume enable initial concentrations
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="989" activeTab="13"/>
+    <workbookView windowWidth="19800" windowHeight="6945" tabRatio="989" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -28,49 +28,49 @@
     <sheet name="References" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$M$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Reactions!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">References!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$J$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="185">
   <si>
     <t>Id</t>
   </si>
@@ -341,18 +341,27 @@
     <t>Type</t>
   </si>
   <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Initial volume, distribution</t>
+  </si>
+  <si>
+    <t>Initial volume, mean</t>
+  </si>
+  <si>
+    <t>Initial volume, standard deviation</t>
+  </si>
+  <si>
+    <t>Volume units</t>
+  </si>
+  <si>
     <t>Density</t>
   </si>
   <si>
     <t>Density units</t>
   </si>
   <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Volume units</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -362,15 +371,21 @@
     <t>physical_3d</t>
   </si>
   <si>
+    <t>mass * density</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>init_mass / init_volume</t>
+  </si>
+  <si>
     <t>g ml^-1</t>
   </si>
   <si>
-    <t>mass * density</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
     <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
   </si>
   <si>
@@ -501,9 +516,6 @@
   </si>
   <si>
     <t>dist-init-conc-specie_1[e]</t>
-  </si>
-  <si>
-    <t>normal</t>
   </si>
   <si>
     <t>M</t>
@@ -776,11 +788,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -817,11 +829,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -837,11 +844,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -861,15 +880,31 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -884,7 +919,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -897,9 +939,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,46 +955,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -978,6 +990,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -990,7 +1038,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,25 +1134,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,127 +1158,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1190,24 +1202,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1219,32 +1213,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1267,6 +1235,50 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1275,140 +1287,140 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1460,6 +1472,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2005,22 +2020,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -2037,16 +2052,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -2058,22 +2073,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="L2" s="16"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -2082,16 +2097,16 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -2099,16 +2114,16 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -2155,19 +2170,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2184,22 +2199,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2207,22 +2222,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2230,22 +2245,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2253,22 +2268,22 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2276,22 +2291,22 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2330,13 +2345,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2353,16 +2368,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2402,13 +2417,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2425,22 +2440,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:8">
       <c r="A2" s="9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2455,7 +2470,7 @@
   <sheetPr/>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2479,16 +2494,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2505,92 +2520,92 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="12" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E2" s="13">
         <v>-3</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="12" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="J2" s="12"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:8">
       <c r="A3" s="12" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E3" s="13">
         <v>-4</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="12" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E4" s="13">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="12" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E5" s="13">
         <v>2</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2632,13 +2647,13 @@
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2655,111 +2670,111 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D2" s="5">
         <v>0.3</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D3" s="7">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D4" s="7">
         <v>0.001</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2800,10 +2815,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2855,28 +2870,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2927,46 +2942,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -3129,23 +3144,23 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:AMM3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1022" width="8.78333333333333" style="5"/>
-    <col min="1023" max="1025" width="8.78333333333333"/>
+    <col min="1" max="1025" width="8.78333333333333" style="5"/>
+    <col min="1026" max="1028" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.1" customHeight="1" spans="1:1024">
+    <row r="1" s="6" customFormat="1" ht="15.1" customHeight="1" spans="1:1027">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3168,78 +3183,105 @@
         <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AMI1"/>
-      <c r="AMJ1"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:10">
+      <c r="AML1"/>
+      <c r="AMM1"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:13">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.09</v>
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="19">
+        <v>4.58e-17</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4.58e-18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:13">
+      <c r="A3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.99318</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J3">
+  <autoFilter ref="A1:M3">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3274,16 +3316,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>37</v>
@@ -3303,14 +3345,14 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -3319,7 +3361,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
@@ -3327,14 +3369,14 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -3343,7 +3385,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -3351,14 +3393,14 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -3367,7 +3409,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
@@ -3375,14 +3417,14 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="10" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -3391,7 +3433,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -3399,14 +3441,14 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="10" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -3415,7 +3457,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
@@ -3423,13 +3465,13 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
       <c r="A7" s="10" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -3438,7 +3480,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
@@ -3480,13 +3522,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -3503,114 +3545,114 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3653,19 +3695,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3682,13 +3724,13 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="E2" s="17">
         <v>0.000148</v>
@@ -3697,20 +3739,20 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="E3" s="17">
         <v>0.0002</v>
@@ -3719,20 +3761,20 @@
         <v>0.014142135623731</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="E4" s="17">
         <v>0.0005</v>
@@ -3741,20 +3783,20 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="E5" s="17">
         <v>0.0005</v>
@@ -3763,20 +3805,20 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="E6" s="17">
         <v>0.001</v>
@@ -3785,20 +3827,20 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="E7" s="17">
         <v>0.002</v>
@@ -3807,7 +3849,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -3845,10 +3887,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -3900,10 +3942,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
adding compartment physical, bioligical types, parents/subcompartments, and convenience methods
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6945" tabRatio="989" activeTab="3"/>
+    <workbookView windowWidth="28200" windowHeight="14070" tabRatio="989" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -28,49 +28,49 @@
     <sheet name="References" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$P$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Reactions!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">References!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$M$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="192">
   <si>
     <t>Id</t>
   </si>
@@ -338,76 +338,97 @@
     <t>ssa</t>
   </si>
   <si>
+    <t>Biological type</t>
+  </si>
+  <si>
+    <t>Physical type</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <t>Parent compartment</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Initial volume, distribution</t>
+  </si>
+  <si>
+    <t>Initial volume, mean</t>
+  </si>
+  <si>
+    <t>Initial volume, standard deviation</t>
+  </si>
+  <si>
+    <t>Volume units</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Density units</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>cellular</t>
+  </si>
+  <si>
+    <t>fluid</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>mass * density</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>init_mass / init_volume</t>
+  </si>
+  <si>
+    <t>g ml^-1</t>
+  </si>
+  <si>
+    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
+  </si>
+  <si>
+    <t>Extracellular space</t>
+  </si>
+  <si>
+    <t>extracellular</t>
+  </si>
+  <si>
+    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1E9 cells/mL [Ref-0002].</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Empirical formula</t>
+  </si>
+  <si>
+    <t>Molecular weight</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Initial volume, distribution</t>
-  </si>
-  <si>
-    <t>Initial volume, mean</t>
-  </si>
-  <si>
-    <t>Initial volume, standard deviation</t>
-  </si>
-  <si>
-    <t>Volume units</t>
-  </si>
-  <si>
-    <t>Density</t>
-  </si>
-  <si>
-    <t>Density units</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>physical_3d</t>
-  </si>
-  <si>
-    <t>mass * density</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>init_mass / init_volume</t>
-  </si>
-  <si>
-    <t>g ml^-1</t>
-  </si>
-  <si>
-    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>Extracellular space</t>
-  </si>
-  <si>
-    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1E9 cells/mL [Ref-0002].</t>
-  </si>
-  <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>Empirical formula</t>
-  </si>
-  <si>
-    <t>Molecular weight</t>
-  </si>
-  <si>
-    <t>Charge</t>
   </si>
   <si>
     <t>specie_1</t>
@@ -790,8 +811,8 @@
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
     <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -829,16 +850,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -849,18 +869,18 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -873,7 +893,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -894,8 +914,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -912,14 +939,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -932,40 +966,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -984,31 +1005,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,7 +1041,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1038,97 +1149,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1140,31 +1185,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1187,17 +1208,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1232,15 +1247,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1252,15 +1258,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1284,135 +1281,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2020,22 +2041,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -2052,16 +2073,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="5" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -2073,22 +2094,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="L2" s="16"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -2097,16 +2118,16 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -2114,16 +2135,16 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -2170,19 +2191,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2199,22 +2220,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2222,22 +2243,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2245,22 +2266,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2268,22 +2289,22 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="F5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2291,22 +2312,22 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2345,13 +2366,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2368,16 +2389,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2417,13 +2438,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2440,22 +2461,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:8">
       <c r="A2" s="9" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2494,16 +2515,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2520,92 +2541,92 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="12" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E2" s="13">
         <v>-3</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="12" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="J2" s="12"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:8">
       <c r="A3" s="12" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E3" s="13">
         <v>-4</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="12" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E4" s="13">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="12" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E5" s="13">
         <v>2</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2644,16 +2665,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2670,111 +2691,111 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D2" s="5">
         <v>0.3</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="5" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D3" s="7">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D4" s="7">
         <v>0.001</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2815,10 +2836,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2870,28 +2891,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2942,46 +2963,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -3144,23 +3165,23 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMM3"/>
+  <dimension ref="A1:AMP3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2:I3"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="5"/>
-    <col min="1026" max="1028" width="8.78333333333333"/>
+    <col min="1" max="1028" width="8.78333333333333" style="5"/>
+    <col min="1029" max="1031" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.1" customHeight="1" spans="1:1027">
+    <row r="1" s="6" customFormat="1" ht="15.1" customHeight="1" spans="1:1030">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3192,96 +3213,120 @@
         <v>44</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AML1"/>
-      <c r="AMM1"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:13">
+      <c r="AMO1"/>
+      <c r="AMP1"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:16">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="19">
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="19">
         <v>4.58e-17</v>
       </c>
-      <c r="G2" s="1">
+      <c r="J2" s="1">
         <v>4.58e-18</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:16">
+      <c r="A3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:13">
-      <c r="A3" s="5" t="s">
+      <c r="G3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="H3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
+      <c r="J3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="5" t="s">
+      <c r="K3" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M3">
+  <autoFilter ref="A1:P3">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3316,19 +3361,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3345,14 +3390,14 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -3361,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
@@ -3369,14 +3414,14 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -3385,7 +3430,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
@@ -3393,14 +3438,14 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -3409,7 +3454,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
@@ -3417,14 +3462,14 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="10" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -3433,7 +3478,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -3441,14 +3486,14 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="10" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -3457,7 +3502,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
@@ -3465,13 +3510,13 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
       <c r="A7" s="10" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -3480,7 +3525,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
@@ -3522,13 +3567,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -3545,114 +3590,114 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3695,19 +3740,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3724,13 +3769,13 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E2" s="17">
         <v>0.000148</v>
@@ -3739,20 +3784,20 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E3" s="17">
         <v>0.0002</v>
@@ -3761,20 +3806,20 @@
         <v>0.014142135623731</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E4" s="17">
         <v>0.0005</v>
@@ -3783,20 +3828,20 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E5" s="17">
         <v>0.0005</v>
@@ -3805,20 +3850,20 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E6" s="17">
         <v>0.001</v>
@@ -3827,20 +3872,20 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E7" s="17">
         <v>0.002</v>
@@ -3849,7 +3894,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -3887,10 +3932,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -3942,10 +3987,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
making reaction rate units composable
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="14070" tabRatio="989" activeTab="3"/>
+    <workbookView windowWidth="28200" windowHeight="13965" tabRatio="989" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="193">
   <si>
     <t>Id</t>
   </si>
@@ -575,7 +575,7 @@
     <t>Flux max</t>
   </si>
   <si>
-    <t>Flux units</t>
+    <t>Flux bound units</t>
   </si>
   <si>
     <t>reaction_1</t>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>k_cat_5 * specie_2[c]</t>
+  </si>
+  <si>
+    <t>Coefficient units</t>
   </si>
   <si>
     <t>dfba-obj-submodel_1</t>
@@ -808,11 +811,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -842,18 +845,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -869,23 +865,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -908,21 +897,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -937,9 +934,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -954,29 +980,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1005,19 +1008,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1035,13 +1032,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1053,7 +1062,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1065,7 +1104,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,115 +1188,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1213,6 +1216,30 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1281,163 +1308,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1486,13 +1489,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2020,7 +2023,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
@@ -2340,14 +2343,14 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2355,10 +2358,10 @@
     <col min="1" max="1" width="25.925" style="1"/>
     <col min="2" max="3" width="9.10833333333333" style="1"/>
     <col min="4" max="4" width="11.3583333333333" style="1"/>
-    <col min="5" max="1025" width="9.10833333333333" style="1"/>
+    <col min="5" max="1026" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
+    <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2375,21 +2378,24 @@
         <v>89</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:5">
+    <row r="2" ht="15.1" customHeight="1" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
@@ -2398,7 +2404,10 @@
         <v>117</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2444,7 +2453,7 @@
         <v>89</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2461,10 +2470,10 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:8">
       <c r="A2" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>30</v>
@@ -2476,7 +2485,7 @@
         <v>56</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2515,13 +2524,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>99</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>89</v>
@@ -2541,13 +2550,13 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>93</v>
@@ -2561,19 +2570,19 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J2" s="12"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:8">
       <c r="A3" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>94</v>
@@ -2589,13 +2598,13 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>95</v>
@@ -2611,13 +2620,13 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>96</v>
@@ -2668,10 +2677,10 @@
         <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>89</v>
@@ -2691,10 +2700,10 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>134</v>
@@ -2704,35 +2713,35 @@
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D3" s="7">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D4" s="7">
         <v>0.001</v>
@@ -2744,24 +2753,24 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
@@ -2772,30 +2781,30 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2891,7 +2900,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>89</v>
@@ -2900,19 +2909,19 @@
         <v>67</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2963,46 +2972,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>67</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -3167,7 +3176,7 @@
   <sheetPr/>
   <dimension ref="A1:AMP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>

</xml_diff>

<commit_message>
clarifying mass, volume, and density calculations
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13965" tabRatio="989" activeTab="11"/>
+    <workbookView windowWidth="28200" windowHeight="13965" tabRatio="989" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -28,49 +28,49 @@
     <sheet name="References" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$O$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Reactions!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">References!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="201">
   <si>
     <t>Id</t>
   </si>
@@ -350,448 +350,469 @@
     <t>Parent compartment</t>
   </si>
   <si>
+    <t>Mass units</t>
+  </si>
+  <si>
+    <t>Initial volume distribution</t>
+  </si>
+  <si>
+    <t>Initial volume mean</t>
+  </si>
+  <si>
+    <t>Initial volume standard deviation</t>
+  </si>
+  <si>
+    <t>Initial volume units</t>
+  </si>
+  <si>
+    <t>Initial density</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>cellular</t>
+  </si>
+  <si>
+    <t>fluid</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>density_c</t>
+  </si>
+  <si>
+    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
+  </si>
+  <si>
+    <t>Extracellular space</t>
+  </si>
+  <si>
+    <t>extracellular</t>
+  </si>
+  <si>
+    <t>density_e</t>
+  </si>
+  <si>
+    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1E9 cells/mL [Ref-0002].</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Empirical formula</t>
+  </si>
+  <si>
+    <t>Molecular weight</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>specie_1</t>
+  </si>
+  <si>
+    <t>specie_name_1</t>
+  </si>
+  <si>
+    <t>NaHCO</t>
+  </si>
+  <si>
+    <t>pseudo_species</t>
+  </si>
+  <si>
+    <t>specie_2</t>
+  </si>
+  <si>
+    <t>specie_name_2</t>
+  </si>
+  <si>
+    <t>N2O2P</t>
+  </si>
+  <si>
+    <t>specie_3</t>
+  </si>
+  <si>
+    <t>specie_name_3</t>
+  </si>
+  <si>
+    <t>N4O4P2</t>
+  </si>
+  <si>
+    <t>specie_4</t>
+  </si>
+  <si>
+    <t>specie_name_4</t>
+  </si>
+  <si>
+    <t>N10O10P5</t>
+  </si>
+  <si>
+    <t>specie_5</t>
+  </si>
+  <si>
+    <t>specie_name_5</t>
+  </si>
+  <si>
+    <t>N5O5</t>
+  </si>
+  <si>
+    <t>specie_6</t>
+  </si>
+  <si>
+    <t>specie_name_6</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>Species type</t>
+  </si>
+  <si>
+    <t>Compartment</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>specie_1[e]</t>
+  </si>
+  <si>
+    <t>molecule</t>
+  </si>
+  <si>
+    <t>specie_2[e]</t>
+  </si>
+  <si>
+    <t>specie_1[c]</t>
+  </si>
+  <si>
+    <t>specie_2[c]</t>
+  </si>
+  <si>
+    <t>specie_3[c]</t>
+  </si>
+  <si>
+    <t>specie_4[c]</t>
+  </si>
+  <si>
+    <t>specie_5[c]</t>
+  </si>
+  <si>
+    <t>specie_6[c]</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_1[e]</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_2[e]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_2[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_4[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_5[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_6[c]</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>volume_c</t>
+  </si>
+  <si>
+    <t>c / density_c</t>
+  </si>
+  <si>
+    <t>volume_e</t>
+  </si>
+  <si>
+    <t>e / density_e</t>
+  </si>
+  <si>
+    <t>Submodel</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Reversible</t>
+  </si>
+  <si>
+    <t>Flux min</t>
+  </si>
+  <si>
+    <t>Flux max</t>
+  </si>
+  <si>
+    <t>Flux bound units</t>
+  </si>
+  <si>
+    <t>reaction_1</t>
+  </si>
+  <si>
+    <t>reaction_name_1</t>
+  </si>
+  <si>
+    <t>specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
+  </si>
+  <si>
+    <t>M s^-1</t>
+  </si>
+  <si>
+    <t>reaction_2</t>
+  </si>
+  <si>
+    <t>reaction_name_2</t>
+  </si>
+  <si>
+    <t>[c]: (2) specie_2 ==&gt; specie_3</t>
+  </si>
+  <si>
+    <t>reaction_3</t>
+  </si>
+  <si>
+    <t>reaction_name_3</t>
+  </si>
+  <si>
+    <t>[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
+  </si>
+  <si>
+    <t>reaction_4</t>
+  </si>
+  <si>
+    <t>reaction_name_4</t>
+  </si>
+  <si>
+    <t>[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
+  </si>
+  <si>
+    <t>Reaction</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>reaction_1-forward</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>k_cat_1 * max( specie_1[e], specie_2[e] )</t>
+  </si>
+  <si>
+    <t>s^-1</t>
+  </si>
+  <si>
+    <t>reaction_2-forward</t>
+  </si>
+  <si>
+    <t>k_cat_2 * specie_2[c]</t>
+  </si>
+  <si>
+    <t>reaction_3-forward</t>
+  </si>
+  <si>
+    <t>k_cat_3_for * specie_4[c] / (specie_4[c] + k_m_3 * Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>reaction_3-backward</t>
+  </si>
+  <si>
+    <t>backward</t>
+  </si>
+  <si>
+    <t>k_cat_3_rev * (specie_5[c] + specie_6[c])</t>
+  </si>
+  <si>
+    <t>reaction_4-forward</t>
+  </si>
+  <si>
+    <t>k_cat_4 * specie_2[c]</t>
+  </si>
+  <si>
+    <t>Reaction rate units</t>
+  </si>
+  <si>
+    <t>Coefficient units</t>
+  </si>
+  <si>
+    <t>dfba-obj-submodel_1</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>Cell size units</t>
+  </si>
+  <si>
+    <t>Metabolism_net_rxn</t>
+  </si>
+  <si>
+    <t>Metabolism net reaction</t>
+  </si>
+  <si>
+    <t>No comment</t>
+  </si>
+  <si>
+    <t>dFBA net reaction</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>dfba-net-species-Metabolism_net_rxn-specie_1[c]</t>
+  </si>
+  <si>
+    <t>dFBA net component 1</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>dfba-net-species-Metabolism_net_rxn-specie_2[c]</t>
+  </si>
+  <si>
+    <t>dFBA net component 2</t>
+  </si>
+  <si>
+    <t>dfba-net-species-Metabolism_net_rxn-specie_3[c]</t>
+  </si>
+  <si>
+    <t>dFBA net component 3</t>
+  </si>
+  <si>
+    <t>dfba-net-species-Metabolism_net_rxn-specie_4[c]</t>
+  </si>
+  <si>
+    <t>dFBA net component 4</t>
+  </si>
+  <si>
+    <t>Standard error</t>
+  </si>
+  <si>
+    <t>fractionDryWeight</t>
+  </si>
+  <si>
+    <t>Fraction of cell mass which is non water</t>
+  </si>
+  <si>
+    <t>[Ref-0006]</t>
+  </si>
+  <si>
+    <t>k_cat_2</t>
+  </si>
+  <si>
+    <t>k_cat</t>
+  </si>
+  <si>
+    <t>molecule^-1 s^-1</t>
+  </si>
+  <si>
+    <t>k_m_3</t>
+  </si>
+  <si>
+    <t>K_m</t>
+  </si>
+  <si>
+    <t>k_cat_1</t>
+  </si>
+  <si>
+    <t>k_cat_3_for</t>
+  </si>
+  <si>
+    <t>k_cat_3_rev</t>
+  </si>
+  <si>
+    <t>k_cat_4</t>
+  </si>
+  <si>
+    <t>g l^-1</t>
+  </si>
+  <si>
+    <t>Avogadro</t>
+  </si>
+  <si>
+    <t>molecule mol^-1</t>
+  </si>
+  <si>
+    <t>Taxon</t>
+  </si>
+  <si>
+    <t>Genetic variant</t>
+  </si>
+  <si>
+    <t>Temperature (C)</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>Growth media</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Editor</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Publication</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
     <t>Volume</t>
-  </si>
-  <si>
-    <t>Initial volume, distribution</t>
-  </si>
-  <si>
-    <t>Initial volume, mean</t>
-  </si>
-  <si>
-    <t>Initial volume, standard deviation</t>
-  </si>
-  <si>
-    <t>Volume units</t>
-  </si>
-  <si>
-    <t>Density</t>
-  </si>
-  <si>
-    <t>Density units</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>cellular</t>
-  </si>
-  <si>
-    <t>fluid</t>
-  </si>
-  <si>
-    <t>3d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>mass * density</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>init_mass / init_volume</t>
-  </si>
-  <si>
-    <t>g ml^-1</t>
-  </si>
-  <si>
-    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
-  </si>
-  <si>
-    <t>Extracellular space</t>
-  </si>
-  <si>
-    <t>extracellular</t>
-  </si>
-  <si>
-    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1E9 cells/mL [Ref-0002].</t>
-  </si>
-  <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>Empirical formula</t>
-  </si>
-  <si>
-    <t>Molecular weight</t>
-  </si>
-  <si>
-    <t>Charge</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>specie_1</t>
-  </si>
-  <si>
-    <t>specie_name_1</t>
-  </si>
-  <si>
-    <t>NaHCO</t>
-  </si>
-  <si>
-    <t>pseudo_species</t>
-  </si>
-  <si>
-    <t>specie_2</t>
-  </si>
-  <si>
-    <t>specie_name_2</t>
-  </si>
-  <si>
-    <t>N2O2P</t>
-  </si>
-  <si>
-    <t>specie_3</t>
-  </si>
-  <si>
-    <t>specie_name_3</t>
-  </si>
-  <si>
-    <t>N4O4P2</t>
-  </si>
-  <si>
-    <t>specie_4</t>
-  </si>
-  <si>
-    <t>specie_name_4</t>
-  </si>
-  <si>
-    <t>N10O10P5</t>
-  </si>
-  <si>
-    <t>specie_5</t>
-  </si>
-  <si>
-    <t>specie_name_5</t>
-  </si>
-  <si>
-    <t>N5O5</t>
-  </si>
-  <si>
-    <t>specie_6</t>
-  </si>
-  <si>
-    <t>specie_name_6</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>Species type</t>
-  </si>
-  <si>
-    <t>Compartment</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>specie_1[e]</t>
-  </si>
-  <si>
-    <t>molecule</t>
-  </si>
-  <si>
-    <t>specie_2[e]</t>
-  </si>
-  <si>
-    <t>specie_1[c]</t>
-  </si>
-  <si>
-    <t>specie_2[c]</t>
-  </si>
-  <si>
-    <t>specie_3[c]</t>
-  </si>
-  <si>
-    <t>specie_4[c]</t>
-  </si>
-  <si>
-    <t>specie_5[c]</t>
-  </si>
-  <si>
-    <t>specie_6[c]</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Distribution</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Standard deviation</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_1[e]</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_2[e]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_2[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_4[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_5[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_6[c]</t>
-  </si>
-  <si>
-    <t>Expression</t>
-  </si>
-  <si>
-    <t>Submodel</t>
-  </si>
-  <si>
-    <t>Participants</t>
-  </si>
-  <si>
-    <t>Reversible</t>
-  </si>
-  <si>
-    <t>Flux min</t>
-  </si>
-  <si>
-    <t>Flux max</t>
-  </si>
-  <si>
-    <t>Flux bound units</t>
-  </si>
-  <si>
-    <t>reaction_1</t>
-  </si>
-  <si>
-    <t>reaction_name_1</t>
-  </si>
-  <si>
-    <t>specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
-  </si>
-  <si>
-    <t>M s^-1</t>
-  </si>
-  <si>
-    <t>reaction_2</t>
-  </si>
-  <si>
-    <t>reaction_name_2</t>
-  </si>
-  <si>
-    <t>[c]: (2) specie_2 ==&gt; specie_3</t>
-  </si>
-  <si>
-    <t>reaction_3</t>
-  </si>
-  <si>
-    <t>reaction_name_3</t>
-  </si>
-  <si>
-    <t>[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
-  </si>
-  <si>
-    <t>reaction_4</t>
-  </si>
-  <si>
-    <t>reaction_name_4</t>
-  </si>
-  <si>
-    <t>[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
-  </si>
-  <si>
-    <t>Reaction</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>reaction_1-forward</t>
-  </si>
-  <si>
-    <t>forward</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>k_cat_1 * max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t>s^-1</t>
-  </si>
-  <si>
-    <t>reaction_2-forward</t>
-  </si>
-  <si>
-    <t>k_cat_2 * specie_2[c]</t>
-  </si>
-  <si>
-    <t>reaction_3-forward</t>
-  </si>
-  <si>
-    <t>k_cat_3 * specie_4[c] / k_m_3</t>
-  </si>
-  <si>
-    <t>reaction_3-backward</t>
-  </si>
-  <si>
-    <t>backward</t>
-  </si>
-  <si>
-    <t>k_cat_4 * (specie_5[c] + specie_6[c])</t>
-  </si>
-  <si>
-    <t>reaction_4-forward</t>
-  </si>
-  <si>
-    <t>k_cat_5 * specie_2[c]</t>
-  </si>
-  <si>
-    <t>Reaction rate units</t>
-  </si>
-  <si>
-    <t>Coefficient units</t>
-  </si>
-  <si>
-    <t>dfba-obj-submodel_1</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>Cell size units</t>
-  </si>
-  <si>
-    <t>Metabolism_net_rxn</t>
-  </si>
-  <si>
-    <t>Metabolism net reaction</t>
-  </si>
-  <si>
-    <t>No comment</t>
-  </si>
-  <si>
-    <t>dFBA net reaction</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>dfba-net-species-Metabolism_net_rxn-specie_1[c]</t>
-  </si>
-  <si>
-    <t>dFBA net component 1</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>dfba-net-species-Metabolism_net_rxn-specie_2[c]</t>
-  </si>
-  <si>
-    <t>dFBA net component 2</t>
-  </si>
-  <si>
-    <t>dfba-net-species-Metabolism_net_rxn-specie_3[c]</t>
-  </si>
-  <si>
-    <t>dFBA net component 3</t>
-  </si>
-  <si>
-    <t>dfba-net-species-Metabolism_net_rxn-specie_4[c]</t>
-  </si>
-  <si>
-    <t>dFBA net component 4</t>
-  </si>
-  <si>
-    <t>Standard error</t>
-  </si>
-  <si>
-    <t>fractionDryWeight</t>
-  </si>
-  <si>
-    <t>Fraction of cell mass which is non water</t>
-  </si>
-  <si>
-    <t>[Ref-0006]</t>
-  </si>
-  <si>
-    <t>k_cat_2</t>
-  </si>
-  <si>
-    <t>k_cat</t>
-  </si>
-  <si>
-    <t>molecule^-1 s^-1</t>
-  </si>
-  <si>
-    <t>k_m_3</t>
-  </si>
-  <si>
-    <t>K_m</t>
-  </si>
-  <si>
-    <t>k_cat_1</t>
-  </si>
-  <si>
-    <t>k_cat_3</t>
-  </si>
-  <si>
-    <t>k_cat_4</t>
-  </si>
-  <si>
-    <t>k_cat_5</t>
-  </si>
-  <si>
-    <t>Taxon</t>
-  </si>
-  <si>
-    <t>Genetic variant</t>
-  </si>
-  <si>
-    <t>Temperature (C)</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>Growth media</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Editor</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Publication</t>
-  </si>
-  <si>
-    <t>Publisher</t>
-  </si>
-  <si>
-    <t>Series</t>
   </si>
   <si>
     <t>Number</t>
@@ -814,11 +835,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -848,6 +869,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -856,46 +885,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -905,8 +904,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -921,31 +935,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -965,22 +965,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -990,6 +982,35 @@
     <font>
       <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1011,7 +1032,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1035,43 +1146,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1083,13 +1164,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1101,97 +1206,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1214,26 +1235,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1270,20 +1276,35 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1307,147 +1328,147 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1468,6 +1489,9 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1492,16 +1516,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2047,22 +2074,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
@@ -2079,16 +2106,16 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -2100,40 +2127,40 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="L2" s="16"/>
+        <v>123</v>
+      </c>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="L3" s="16"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -2141,16 +2168,16 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>129</v>
+      <c r="D5" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -2176,15 +2203,17 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="16.3916666666667" style="1"/>
-    <col min="2" max="4" width="8.78333333333333" style="1"/>
-    <col min="5" max="5" width="4.5" style="1"/>
-    <col min="6" max="6" width="27.425" style="1"/>
+    <col min="1" max="1" width="17.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.78333333333333" style="1"/>
+    <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="60.375" style="1" customWidth="1"/>
     <col min="7" max="1023" width="8.78333333333333" style="1"/>
     <col min="1024" max="1025" width="8.78333333333333"/>
   </cols>
@@ -2197,19 +2226,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2226,22 +2255,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2249,22 +2278,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2272,22 +2301,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2295,22 +2324,22 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2318,22 +2347,22 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2348,7 +2377,7 @@
   <sheetPr/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2372,19 +2401,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2401,19 +2430,19 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -2444,25 +2473,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="9" width="8.78333333333333" style="9"/>
-    <col min="10" max="1025" width="8.78333333333333" style="10"/>
+    <col min="1" max="9" width="8.78333333333333" style="10"/>
+    <col min="10" max="1025" width="8.78333333333333" style="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>150</v>
+      <c r="C1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2470,31 +2499,31 @@
       <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:8">
-      <c r="A2" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>153</v>
+      <c r="D2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2519,30 +2548,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="5" width="8.78333333333333" style="9"/>
+    <col min="1" max="5" width="8.78333333333333" style="10"/>
     <col min="6" max="6" width="8.78333333333333" style="4"/>
-    <col min="7" max="10" width="8.78333333333333" style="9"/>
-    <col min="11" max="1025" width="8.78333333333333" style="10"/>
+    <col min="7" max="10" width="8.78333333333333" style="10"/>
+    <col min="11" max="1025" width="8.78333333333333" style="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>89</v>
+      <c r="C1" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2550,101 +2579,101 @@
       <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A2" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>151</v>
+      <c r="A2" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="13">
+        <v>92</v>
+      </c>
+      <c r="E2" s="14">
         <v>-3</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>120</v>
+      <c r="F2" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="J2" s="12"/>
+      <c r="I2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:8">
-      <c r="A3" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>151</v>
+      <c r="A3" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="13">
+        <v>93</v>
+      </c>
+      <c r="E3" s="14">
         <v>-4</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>120</v>
+      <c r="F3" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
-      <c r="A4" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>151</v>
+      <c r="A4" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="13">
+        <v>94</v>
+      </c>
+      <c r="E4" s="14">
         <v>1</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>120</v>
+      <c r="F4" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A5" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="13">
+      <c r="A5" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="14">
         <v>2</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>120</v>
+      <c r="F5" s="15" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2657,17 +2686,17 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K34" sqref="K34"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="5" width="8.78333333333333" style="5"/>
     <col min="6" max="6" width="16.175" style="5"/>
@@ -2683,16 +2712,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2709,111 +2738,159 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D2" s="5">
         <v>0.3</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D3" s="7">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D4" s="7">
         <v>0.001</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="8">
+        <v>6.02214075862e+23</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2831,7 +2908,7 @@
   <sheetPr/>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2854,10 +2931,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2909,28 +2986,28 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -2981,46 +3058,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -3052,14 +3129,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="10"/>
+    <col min="1" max="1025" width="8.78333333333333" style="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3067,7 +3144,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3075,7 +3152,7 @@
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3089,7 +3166,7 @@
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3183,23 +3260,23 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMP3"/>
+  <dimension ref="A1:AMO3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1028" width="8.78333333333333" style="5"/>
-    <col min="1029" max="1031" width="8.78333333333333"/>
+    <col min="1" max="1027" width="8.78333333333333" style="5"/>
+    <col min="1028" max="1030" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.1" customHeight="1" spans="1:1030">
+    <row r="1" s="6" customFormat="1" ht="15.1" customHeight="1" spans="1:1029">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3237,90 +3314,84 @@
         <v>46</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AMN1"/>
+      <c r="AMO1"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:15">
+      <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AMO1"/>
-      <c r="AMP1"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:16">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="19">
+      <c r="I2" s="8">
         <v>4.58e-17</v>
       </c>
       <c r="J2" s="1">
         <v>4.58e-18</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="1" t="s">
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:15">
+      <c r="A3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:16">
-      <c r="A3" s="5" t="s">
+      <c r="D3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -3329,22 +3400,19 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="5" t="s">
-        <v>62</v>
+      <c r="O3" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P3">
+  <autoFilter ref="A1:O3">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3379,19 +3447,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3408,14 +3476,14 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -3423,23 +3491,23 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="G2" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -3447,23 +3515,23 @@
       <c r="F3" s="1">
         <v>-1</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="G3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -3471,23 +3539,23 @@
       <c r="F4" s="1">
         <v>-2</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="G4" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -3495,23 +3563,23 @@
       <c r="F5" s="1">
         <v>-5</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
+      <c r="G5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -3519,22 +3587,22 @@
       <c r="F6" s="1">
         <v>-3</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="G6" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="D7" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -3542,11 +3610,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="G7" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K7">
@@ -3585,13 +3653,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -3608,114 +3676,114 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3758,19 +3826,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -3787,135 +3855,135 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="20">
+        <v>0.000148</v>
+      </c>
+      <c r="F2" s="20">
+        <v>0.0121655250605964</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="17">
-        <v>0.000148</v>
-      </c>
-      <c r="F2" s="17">
-        <v>0.0121655250605964</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="17">
+        <v>54</v>
+      </c>
+      <c r="E3" s="20">
         <v>0.0002</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="20">
         <v>0.014142135623731</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="G3" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="17">
+        <v>54</v>
+      </c>
+      <c r="E4" s="20">
         <v>0.0005</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="20">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="G4" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="17">
+        <v>54</v>
+      </c>
+      <c r="E5" s="20">
         <v>0.0005</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="20">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="G5" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="17">
+        <v>54</v>
+      </c>
+      <c r="E6" s="20">
         <v>0.001</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="20">
         <v>0.0316227766016838</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="G6" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="17">
+        <v>54</v>
+      </c>
+      <c r="E7" s="20">
         <v>0.002</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="20">
         <v>0.0447213595499958</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="G7" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3950,10 +4018,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -3981,23 +4049,27 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P36" sqref="P36"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1023" width="8.78333333333333" style="4"/>
-    <col min="1024" max="1025" width="8.78333333333333"/>
+    <col min="1" max="1" width="8.5" style="18" customWidth="1"/>
+    <col min="2" max="2" width="8.78333333333333" style="18"/>
+    <col min="3" max="3" width="11" style="18" customWidth="1"/>
+    <col min="4" max="1023" width="8.78333333333333" style="18"/>
+    <col min="1024" max="1025" width="8.78333333333333" style="19"/>
+    <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:8">
+    <row r="1" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4005,10 +4077,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -4021,6 +4093,30 @@
       </c>
       <c r="H1" s="2" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting to factor expression module out of wc_lang to obj_model
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13965" tabRatio="989" activeTab="15"/>
+    <workbookView windowWidth="28200" windowHeight="14070" tabRatio="989" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$O$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">References!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!#REF!</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="202">
   <si>
     <t>Id</t>
   </si>
@@ -578,6 +578,9 @@
     <t>Reversible</t>
   </si>
   <si>
+    <t>Rate units</t>
+  </si>
+  <si>
     <t>Flux min</t>
   </si>
   <si>
@@ -596,6 +599,9 @@
     <t>specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
   </si>
   <si>
+    <t>s^-1</t>
+  </si>
+  <si>
     <t>M s^-1</t>
   </si>
   <si>
@@ -642,9 +648,6 @@
   </si>
   <si>
     <t>k_cat_1 * max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t>s^-1</t>
   </si>
   <si>
     <t>reaction_2-forward</t>
@@ -836,11 +839,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -877,6 +880,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -885,16 +893,25 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -906,7 +923,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -922,29 +946,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -959,7 +960,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -967,7 +968,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -981,31 +1005,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1032,7 +1035,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1044,7 +1059,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,31 +1071,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1098,13 +1149,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1116,73 +1197,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1194,25 +1215,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1235,11 +1238,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1255,6 +1264,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1285,17 +1309,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1308,167 +1335,143 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1518,9 +1521,6 @@
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2046,14 +2046,14 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
@@ -2062,11 +2062,11 @@
     <col min="2" max="2" width="13.3916666666667" style="5"/>
     <col min="3" max="3" width="10.3916666666667" style="5"/>
     <col min="4" max="4" width="49.4916666666667" style="5"/>
-    <col min="5" max="12" width="8.78333333333333" style="5"/>
-    <col min="13" max="1025" width="8.78333333333333" style="6"/>
+    <col min="5" max="13" width="8.78333333333333" style="5"/>
+    <col min="14" max="1026" width="8.78333333333333" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:12">
+    <row r="1" ht="15.1" customHeight="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2092,95 +2092,110 @@
         <v>119</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:12">
+    <row r="2" ht="15.1" customHeight="1" spans="1:13">
       <c r="A2" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="5">
         <v>0</v>
       </c>
-      <c r="G2" s="5">
+      <c r="H2" s="5">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:12">
+      <c r="I2" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:13">
       <c r="A3" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="L3" s="17"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:5">
+      <c r="F3" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:5">
+      <c r="F4" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2226,10 +2241,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>66</v>
@@ -2255,22 +2270,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2278,22 +2293,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2301,22 +2316,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2324,22 +2339,22 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2347,22 +2362,22 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2410,10 +2425,10 @@
         <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2430,19 +2445,19 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -2491,7 +2506,7 @@
         <v>88</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2508,22 +2523,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:8">
       <c r="A2" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>55</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2562,13 +2577,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>98</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>88</v>
@@ -2588,13 +2603,13 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>92</v>
@@ -2603,24 +2618,24 @@
         <v>-3</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J2" s="13"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:8">
       <c r="A3" s="13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>93</v>
@@ -2629,20 +2644,20 @@
         <v>-4</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>94</v>
@@ -2651,20 +2666,20 @@
         <v>1</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>95</v>
@@ -2673,7 +2688,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2715,10 +2730,10 @@
         <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>88</v>
@@ -2738,48 +2753,48 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D2" s="5">
         <v>0.3</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D3" s="7">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D4" s="7">
         <v>0.001</v>
@@ -2791,58 +2806,58 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2851,14 +2866,14 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D9" s="1">
         <v>1100</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2867,34 +2882,34 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D10" s="1">
         <v>1100</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D11" s="8">
         <v>6.02214075862e+23</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F8">
+  <autoFilter ref="A1:F11">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2908,7 +2923,7 @@
   <sheetPr/>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2986,7 +3001,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>88</v>
@@ -2995,19 +3010,19 @@
         <v>66</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
@@ -3058,46 +3073,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -3491,12 +3506,12 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
@@ -3515,12 +3530,12 @@
       <c r="F3" s="1">
         <v>-1</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
@@ -3539,12 +3554,12 @@
       <c r="F4" s="1">
         <v>-2</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="11" t="s">
@@ -3563,12 +3578,12 @@
       <c r="F5" s="1">
         <v>-5</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="11" t="s">
@@ -3587,12 +3602,12 @@
       <c r="F6" s="1">
         <v>-3</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
       <c r="A7" s="11" t="s">
@@ -3610,11 +3625,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K7">
@@ -3863,17 +3878,17 @@
       <c r="D2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="19">
         <v>0.000148</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="19">
         <v>0.0121655250605964</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:9">
       <c r="A3" s="4" t="s">
@@ -3885,17 +3900,17 @@
       <c r="D3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="19">
         <v>0.0002</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="19">
         <v>0.014142135623731</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:9">
       <c r="A4" s="4" t="s">
@@ -3907,17 +3922,17 @@
       <c r="D4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
         <v>0.0005</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="19">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:9">
       <c r="A5" s="4" t="s">
@@ -3929,17 +3944,17 @@
       <c r="D5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="19">
         <v>0.0005</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="19">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:9">
       <c r="A6" s="4" t="s">
@@ -3951,17 +3966,17 @@
       <c r="D6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <v>0.001</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="19">
         <v>0.0316227766016838</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:9">
       <c r="A7" s="4" t="s">
@@ -3973,17 +3988,17 @@
       <c r="D7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="19">
         <v>0.002</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="19">
         <v>0.0447213595499958</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4061,12 +4076,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="18" customWidth="1"/>
-    <col min="2" max="2" width="8.78333333333333" style="18"/>
-    <col min="3" max="3" width="11" style="18" customWidth="1"/>
-    <col min="4" max="1023" width="8.78333333333333" style="18"/>
-    <col min="1024" max="1025" width="8.78333333333333" style="19"/>
-    <col min="1026" max="16384" width="9" style="19"/>
+    <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.78333333333333" style="1"/>
+    <col min="3" max="3" width="11" style="1" customWidth="1"/>
+    <col min="4" max="1023" width="8.78333333333333" style="1"/>
+    <col min="1024" max="1025" width="8.78333333333333" style="18"/>
+    <col min="1026" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:8">
@@ -4099,7 +4114,6 @@
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>111</v>
       </c>
@@ -4111,7 +4125,6 @@
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
adding class to represent environment
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,227 +5,228 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="14070" tabRatio="989" activeTab="9"/>
+    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
     <sheet name="Taxon" sheetId="2" r:id="rId2"/>
-    <sheet name="Submodels" sheetId="3" r:id="rId3"/>
-    <sheet name="Compartments" sheetId="4" r:id="rId4"/>
-    <sheet name="Species types" sheetId="5" r:id="rId5"/>
-    <sheet name="Species" sheetId="6" r:id="rId6"/>
-    <sheet name="Initial species concentrations" sheetId="7" r:id="rId7"/>
-    <sheet name="Observables" sheetId="8" r:id="rId8"/>
-    <sheet name="Functions" sheetId="9" r:id="rId9"/>
-    <sheet name="Reactions" sheetId="10" r:id="rId10"/>
-    <sheet name="Rate laws" sheetId="11" r:id="rId11"/>
-    <sheet name="dFBA objectives" sheetId="12" r:id="rId12"/>
-    <sheet name="dFBA net reactions" sheetId="13" r:id="rId13"/>
-    <sheet name="dFBA net species" sheetId="14" r:id="rId14"/>
-    <sheet name="Parameters" sheetId="15" r:id="rId15"/>
-    <sheet name="Stop conditions" sheetId="16" r:id="rId16"/>
-    <sheet name="Evidence" sheetId="17" r:id="rId17"/>
-    <sheet name="References" sheetId="18" r:id="rId18"/>
+    <sheet name="Environment" sheetId="19" r:id="rId3"/>
+    <sheet name="Submodels" sheetId="3" r:id="rId4"/>
+    <sheet name="Compartments" sheetId="4" r:id="rId5"/>
+    <sheet name="Species types" sheetId="5" r:id="rId6"/>
+    <sheet name="Species" sheetId="6" r:id="rId7"/>
+    <sheet name="Initial species concentrations" sheetId="7" r:id="rId8"/>
+    <sheet name="Observables" sheetId="8" r:id="rId9"/>
+    <sheet name="Functions" sheetId="9" r:id="rId10"/>
+    <sheet name="Reactions" sheetId="10" r:id="rId11"/>
+    <sheet name="Rate laws" sheetId="11" r:id="rId12"/>
+    <sheet name="dFBA objectives" sheetId="12" r:id="rId13"/>
+    <sheet name="dFBA net reactions" sheetId="13" r:id="rId14"/>
+    <sheet name="dFBA net species" sheetId="14" r:id="rId15"/>
+    <sheet name="Parameters" sheetId="15" r:id="rId16"/>
+    <sheet name="Stop conditions" sheetId="16" r:id="rId17"/>
+    <sheet name="Evidence" sheetId="17" r:id="rId18"/>
+    <sheet name="References" sheetId="18" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$K$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Parameters!$A$1:$F$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">References!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="3">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="9">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="14">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="17">References!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$K$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">References!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">Submodels!#REF!</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="206">
   <si>
     <t>Id</t>
   </si>
@@ -293,7 +294,7 @@
     <t>Updated</t>
   </si>
   <si>
-    <t>ASP_test</t>
+    <t>taxon</t>
   </si>
   <si>
     <t>Test model for TestExecutableModel</t>
@@ -311,6 +312,21 @@
     <t>References</t>
   </si>
   <si>
+    <t>env</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Temperature units</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
     <t>Algorithm</t>
   </si>
   <si>
@@ -789,9 +805,6 @@
   </si>
   <si>
     <t>Temperature (C)</t>
-  </si>
-  <si>
-    <t>pH</t>
   </si>
   <si>
     <t>Growth media</t>
@@ -838,12 +851,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -872,9 +885,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -893,24 +912,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -930,45 +935,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -981,8 +956,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -997,6 +995,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1005,18 +1019,17 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1035,19 +1048,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,19 +1078,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1095,7 +1108,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1107,31 +1174,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1143,19 +1192,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1167,55 +1228,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1238,32 +1251,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1298,6 +1290,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1312,8 +1319,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1322,156 +1344,147 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1519,17 +1532,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2046,9 +2068,90 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.78333333333333" style="1"/>
+    <col min="3" max="3" width="11" style="1" customWidth="1"/>
+    <col min="4" max="1023" width="8.78333333333333" style="1"/>
+    <col min="1024" max="1025" width="8.78333333333333" style="18"/>
+    <col min="1026" max="16384" width="9" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2074,31 +2177,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>19</v>
@@ -2109,22 +2212,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:13">
       <c r="A2" s="5" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G2" s="5">
         <v>0</v>
@@ -2133,69 +2236,69 @@
         <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="M2" s="17"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:13">
       <c r="A3" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="M3" s="17"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2208,7 +2311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K6"/>
@@ -2241,25 +2344,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>19</v>
@@ -2270,22 +2373,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2293,22 +2396,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2316,22 +2419,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2339,22 +2442,22 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2362,22 +2465,22 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2387,7 +2490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K2"/>
@@ -2416,25 +2519,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>19</v>
@@ -2445,19 +2548,19 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -2473,7 +2576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I2"/>
@@ -2500,19 +2603,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>19</v>
@@ -2523,22 +2626,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:8">
       <c r="A2" s="10" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2548,7 +2651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:J5"/>
@@ -2577,22 +2680,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>19</v>
@@ -2603,92 +2706,92 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>155</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E2" s="14">
         <v>-3</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="13" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="J2" s="13"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:8">
       <c r="A3" s="13" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E3" s="14">
         <v>-4</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="13" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E4" s="14">
         <v>1</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="13" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E5" s="14">
         <v>2</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2698,7 +2801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:J11"/>
@@ -2727,22 +2830,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>19</v>
@@ -2753,159 +2856,159 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D2" s="5">
         <v>0.3</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="5" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D3" s="7">
         <v>2000</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D4" s="7">
         <v>0.001</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D9" s="1">
         <v>1100</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D10" s="1">
         <v>1100</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D11" s="8">
         <v>6.02214075862e+23</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2918,7 +3021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H1"/>
@@ -2946,16 +3049,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>19</v>
@@ -2974,7 +3077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:N1"/>
@@ -3001,34 +3104,34 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>188</v>
+        <v>32</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>19</v>
@@ -3047,7 +3150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:R1"/>
@@ -3073,46 +3176,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -3139,19 +3242,20 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="C9" sqref="C9"/>
+      <selection pane="topRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="11"/>
+    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1026" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3159,7 +3263,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3167,7 +3271,7 @@
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3175,13 +3279,13 @@
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="23"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3198,6 +3302,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="7" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
+    <col min="3" max="1015" width="8.78333333333333" style="1"/>
+    <col min="1016" max="16384" width="9" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:1">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AMJ3"/>
@@ -3224,13 +3405,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>19</v>
@@ -3242,27 +3423,27 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3272,7 +3453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AMO3"/>
@@ -3299,40 +3480,40 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>19</v>
@@ -3345,28 +3526,28 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:15">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I2" s="8">
         <v>4.58e-17</v>
@@ -3375,38 +3556,38 @@
         <v>4.58e-18</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:15">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -3415,15 +3596,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3436,7 +3617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K7"/>
@@ -3462,25 +3643,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>19</v>
@@ -3491,14 +3672,14 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -3507,7 +3688,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -3515,14 +3696,14 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -3531,7 +3712,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -3539,14 +3720,14 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -3555,7 +3736,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -3563,14 +3744,14 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -3579,7 +3760,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -3587,14 +3768,14 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="11" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -3603,7 +3784,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -3611,13 +3792,13 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:9">
       <c r="A7" s="11" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -3626,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
@@ -3641,7 +3822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I9"/>
@@ -3668,19 +3849,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>19</v>
@@ -3691,114 +3872,114 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3811,7 +3992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K7"/>
@@ -3841,25 +4022,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>19</v>
@@ -3870,13 +4051,13 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E2" s="19">
         <v>0.000148</v>
@@ -3885,20 +4066,20 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E3" s="19">
         <v>0.0002</v>
@@ -3907,20 +4088,20 @@
         <v>0.014142135623731</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E4" s="19">
         <v>0.0005</v>
@@ -3929,20 +4110,20 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E5" s="19">
         <v>0.0005</v>
@@ -3951,20 +4132,20 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E6" s="19">
         <v>0.001</v>
@@ -3973,20 +4154,20 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E7" s="19">
         <v>0.002</v>
@@ -3995,7 +4176,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -4007,7 +4188,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H1"/>
@@ -4033,103 +4214,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.78333333333333" style="1"/>
-    <col min="3" max="3" width="11" style="1" customWidth="1"/>
-    <col min="4" max="1023" width="8.78333333333333" style="1"/>
-    <col min="1024" max="1025" width="8.78333333333333" style="18"/>
-    <col min="1026" max="16384" width="9" style="18"/>
-  </cols>
-  <sheetData>
-    <row r="1" customHeight="1" spans="1:8">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding attributes for evidence; adding interpretations; getting test coverage to 100%
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="989" activeTab="2"/>
+    <workbookView windowWidth="19800" windowHeight="6945" tabRatio="989" firstSheet="11" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -26,89 +26,90 @@
     <sheet name="Parameters" sheetId="15" r:id="rId16"/>
     <sheet name="Stop conditions" sheetId="16" r:id="rId17"/>
     <sheet name="Evidence" sheetId="17" r:id="rId18"/>
-    <sheet name="References" sheetId="18" r:id="rId19"/>
+    <sheet name="Interpretations" sheetId="20" r:id="rId19"/>
+    <sheet name="References" sheetId="18" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$K$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$L$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Reactions!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$F$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">References!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">References!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$O$3</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$K$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$1:$P$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="10">Reactions!$A$1:$D$5</definedName>
@@ -183,50 +184,50 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="18">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="213">
   <si>
     <t>Id</t>
   </si>
@@ -339,6 +340,9 @@
     <t>Evidence</t>
   </si>
   <si>
+    <t>Interpretations</t>
+  </si>
+  <si>
     <t>submodel_1</t>
   </si>
   <si>
@@ -807,10 +811,25 @@
     <t>Genetic variant</t>
   </si>
   <si>
-    <t>Temperature (C)</t>
-  </si>
-  <si>
     <t>Growth media</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Experiment type</t>
+  </si>
+  <si>
+    <t>Experiment design</t>
+  </si>
+  <si>
+    <t>Measurement method</t>
+  </si>
+  <si>
+    <t>Analysis method</t>
+  </si>
+  <si>
+    <t>Method</t>
   </si>
   <si>
     <t>Title</t>
@@ -854,12 +873,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -902,14 +921,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -919,14 +953,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -947,17 +973,16 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -969,30 +994,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1006,9 +1010,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1022,6 +1025,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -1030,9 +1041,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1051,132 +1070,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1189,7 +1082,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1201,13 +1178,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1219,19 +1220,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1254,11 +1273,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1302,17 +1327,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1330,156 +1344,161 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1487,7 +1506,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1498,6 +1517,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1535,16 +1557,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2065,27 +2087,27 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.78333333333333" style="1"/>
     <col min="3" max="3" width="11" style="1" customWidth="1"/>
-    <col min="4" max="1023" width="8.78333333333333" style="1"/>
-    <col min="1024" max="1025" width="8.78333333333333" style="18"/>
-    <col min="1026" max="16384" width="9" style="18"/>
+    <col min="4" max="1024" width="8.78333333333333" style="1"/>
+    <col min="1025" max="1026" width="8.78333333333333" style="19"/>
+    <col min="1027" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:8">
+    <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2093,10 +2115,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -2105,32 +2127,35 @@
         <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2146,27 +2171,27 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2:F5"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="8.78333333333333" style="5"/>
-    <col min="2" max="2" width="13.3916666666667" style="5"/>
-    <col min="3" max="3" width="10.3916666666667" style="5"/>
-    <col min="4" max="4" width="49.4916666666667" style="5"/>
-    <col min="5" max="13" width="8.78333333333333" style="5"/>
-    <col min="14" max="1026" width="8.78333333333333" style="6"/>
+    <col min="1" max="1" width="8.78333333333333" style="6"/>
+    <col min="2" max="2" width="13.3916666666667" style="6"/>
+    <col min="3" max="3" width="10.3916666666667" style="6"/>
+    <col min="4" max="4" width="49.4916666666667" style="6"/>
+    <col min="5" max="14" width="8.78333333333333" style="6"/>
+    <col min="15" max="1027" width="8.78333333333333" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:13">
+    <row r="1" ht="15.1" customHeight="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2174,25 +2199,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>18</v>
@@ -2201,101 +2226,104 @@
         <v>36</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:13">
-      <c r="A2" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" ht="15.1" customHeight="1" spans="1:14">
+      <c r="A2" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="5">
+      <c r="C2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="6">
         <v>0</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="F2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="6">
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="N2" s="18"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:14">
+      <c r="A3" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="M2" s="17"/>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:13">
-      <c r="A3" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="N3" s="18"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:6">
+      <c r="A4" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="M3" s="17"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A4" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>131</v>
+      <c r="F4" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="B5" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="5">
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="6">
         <v>0</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>131</v>
+      <c r="F5" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2311,14 +2339,14 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2329,11 +2357,11 @@
     <col min="4" max="4" width="8.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="4.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="60.375" style="1" customWidth="1"/>
-    <col min="7" max="1023" width="8.78333333333333" style="1"/>
-    <col min="1024" max="1025" width="8.78333333333333"/>
+    <col min="7" max="1024" width="8.78333333333333" style="1"/>
+    <col min="1025" max="1026" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2341,19 +2369,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2362,122 +2390,129 @@
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:11">
+    <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:11">
+      <c r="L2"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:11">
+      <c r="L3"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:11">
+      <c r="L4"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
+      <c r="L5"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2490,14 +2525,14 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1:F2"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2505,10 +2540,10 @@
     <col min="1" max="1" width="25.925" style="1"/>
     <col min="2" max="3" width="9.10833333333333" style="1"/>
     <col min="4" max="4" width="11.3583333333333" style="1"/>
-    <col min="5" max="1027" width="9.10833333333333" style="1"/>
+    <col min="5" max="1028" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2516,19 +2551,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2537,27 +2572,30 @@
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -2576,37 +2614,37 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="9" width="8.78333333333333" style="10"/>
-    <col min="10" max="1025" width="8.78333333333333" style="11"/>
+    <col min="1" max="10" width="8.78333333333333" style="11"/>
+    <col min="11" max="1026" width="8.78333333333333" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A1" s="12" t="s">
+    <row r="1" ht="15.1" customHeight="1" spans="1:10">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>160</v>
+      <c r="C1" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2614,31 +2652,34 @@
       <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:8">
-      <c r="A2" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    <row r="2" ht="15.1" customHeight="1" spans="1:9">
+      <c r="A2" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>163</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2651,42 +2692,42 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="5" width="8.78333333333333" style="10"/>
-    <col min="6" max="6" width="8.78333333333333" style="4"/>
-    <col min="7" max="10" width="8.78333333333333" style="10"/>
-    <col min="11" max="1025" width="8.78333333333333" style="11"/>
+    <col min="1" max="5" width="8.78333333333333" style="11"/>
+    <col min="6" max="6" width="8.78333333333333" style="5"/>
+    <col min="7" max="11" width="8.78333333333333" style="11"/>
+    <col min="12" max="1026" width="8.78333333333333" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A1" s="12" t="s">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>95</v>
+      <c r="D1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2694,101 +2735,107 @@
       <c r="H1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A2" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    <row r="2" ht="15.1" customHeight="1" spans="1:11">
+      <c r="A2" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>161</v>
+      <c r="B2" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="14">
+        <v>100</v>
+      </c>
+      <c r="E2" s="15">
         <v>-3</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>132</v>
+      <c r="F2" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:8">
-      <c r="A3" s="13" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:9">
+      <c r="A3" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>161</v>
+      <c r="B3" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="14">
+        <v>101</v>
+      </c>
+      <c r="E3" s="15">
         <v>-4</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>132</v>
+      <c r="F3" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:8">
-      <c r="A4" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:9">
+      <c r="A4" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>161</v>
+      <c r="B4" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="14">
+        <v>102</v>
+      </c>
+      <c r="E4" s="15">
         <v>1</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>132</v>
+      <c r="F4" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A5" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="14">
+      <c r="B5" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="15">
         <v>2</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>132</v>
+      <c r="F5" s="16" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2801,25 +2848,25 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="5" width="8.78333333333333" style="5"/>
-    <col min="6" max="6" width="16.175" style="5"/>
-    <col min="7" max="10" width="8.78333333333333" style="5"/>
-    <col min="11" max="1025" width="8.78333333333333" style="6"/>
+    <col min="1" max="5" width="8.78333333333333" style="6"/>
+    <col min="6" max="6" width="16.175" style="6"/>
+    <col min="7" max="11" width="8.78333333333333" style="6"/>
+    <col min="12" max="1026" width="8.78333333333333" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:10">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2827,16 +2874,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>18</v>
@@ -2845,167 +2892,170 @@
         <v>36</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A2" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" ht="15.1" customHeight="1" spans="1:10">
+      <c r="A2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="B2" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="6">
         <v>0.3</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>178</v>
+      <c r="J2" s="6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A3" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="7">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="8">
         <v>2000</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.001</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:6">
+      <c r="A5" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A4" s="6" t="s">
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.001</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="5">
+    </row>
+    <row r="6" ht="15.1" customHeight="1" spans="1:6">
+      <c r="A6" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F6" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" ht="15.1" customHeight="1" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A6" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="D7" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A7" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="F7" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" ht="15.1" customHeight="1" spans="1:6">
+      <c r="A8" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A8" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>181</v>
+      <c r="F8" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" s="1">
         <v>1100</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D10" s="1">
         <v>1100</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="8">
+        <v>147</v>
+      </c>
+      <c r="D11" s="9">
         <v>6.02214075862e+23</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3021,24 +3071,24 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1022" width="8.78333333333333" style="1"/>
-    <col min="1023" max="1023" width="8.78333333333333" style="4"/>
-    <col min="1024" max="1025" width="8.78333333333333"/>
+    <col min="1" max="1023" width="8.78333333333333" style="1"/>
+    <col min="1024" max="1024" width="8.78333333333333" style="5"/>
+    <col min="1025" max="1026" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:8">
+    <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3046,10 +3096,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -3058,9 +3108,12 @@
         <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3077,23 +3130,23 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:AMS1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q36" sqref="Q36"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="13.3916666666667" style="1"/>
-    <col min="3" max="1025" width="9.10833333333333" style="1"/>
+    <col min="3" max="1030" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:14">
+    <row r="1" ht="15.1" customHeight="1" spans="1:1033">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3101,16 +3154,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>191</v>
+        <v>74</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>192</v>
@@ -3119,23 +3172,50 @@
         <v>193</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AMQ1" s="1"/>
+      <c r="AMR1" s="1"/>
+      <c r="AMS1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3150,84 +3230,98 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S36" sqref="S36"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1" width="15.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" style="1" customWidth="1"/>
+    <col min="3" max="1022" width="9.10833333333333" style="1"/>
+    <col min="1023" max="1023" width="9.10833333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:18">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="I1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" ht="15.1" customHeight="1" spans="3:4">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3245,7 +3339,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1025" width="8.78333333333333" style="1"/>
-    <col min="1026" max="16384" width="9" style="9"/>
+    <col min="1026" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:2">
@@ -3276,7 +3370,7 @@
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:2">
       <c r="A5" s="2" t="s">
@@ -3292,6 +3386,90 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.1" customHeight="1" spans="1:18">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
@@ -3303,10 +3481,10 @@
   <sheetPr/>
   <dimension ref="A1:AMD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A6" sqref="$A6:$XFD6"/>
+      <selection pane="topRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -3314,7 +3492,7 @@
     <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="1015" width="8.78333333333333" style="1"/>
-    <col min="1016" max="16384" width="9" style="11"/>
+    <col min="1016" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:2">
@@ -3354,7 +3532,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="6" s="21" customFormat="1" customHeight="1" spans="1:1018">
+    <row r="6" s="22" customFormat="1" customHeight="1" spans="1:1018">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -4402,23 +4580,23 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1022" width="8.78333333333333" style="5"/>
-    <col min="1023" max="1025" width="8.78333333333333" style="4"/>
+    <col min="1" max="1023" width="8.78333333333333" style="6"/>
+    <col min="1024" max="1026" width="8.78333333333333" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.1" customHeight="1" spans="1:1024">
+    <row r="1" s="7" customFormat="1" ht="15.1" customHeight="1" spans="1:1025">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4435,36 +4613,39 @@
         <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AMJ1" s="4"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:6">
-      <c r="A2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="AMK1" s="5"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:7">
+      <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="G2" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>43</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4477,23 +4658,25 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMO3"/>
+  <dimension ref="A1:AMP3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1027" width="8.78333333333333" style="5"/>
-    <col min="1028" max="1030" width="8.78333333333333"/>
+    <col min="1" max="13" width="8.78333333333333" style="6"/>
+    <col min="14" max="15" width="8.875" style="6" customWidth="1"/>
+    <col min="16" max="1028" width="8.78333333333333" style="6"/>
+    <col min="1029" max="1031" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.1" customHeight="1" spans="1:1029">
+    <row r="1" s="7" customFormat="1" ht="15.1" customHeight="1" spans="1:1030">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4501,34 +4684,34 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>18</v>
@@ -4537,78 +4720,82 @@
         <v>36</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AMN1"/>
       <c r="AMO1"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:15">
-      <c r="A2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="AMP1"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:16">
+      <c r="A2" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="F2" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="8">
+        <v>62</v>
+      </c>
+      <c r="I2" s="9">
         <v>4.58e-17</v>
       </c>
       <c r="J2" s="1">
         <v>4.58e-18</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:16">
+      <c r="A3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:15">
-      <c r="A3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -4617,19 +4804,20 @@
         <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="5" t="s">
         <v>68</v>
       </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O3">
+  <autoFilter ref="A1:P3">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4641,22 +4829,22 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4664,19 +4852,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -4685,22 +4873,25 @@
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:10">
+    <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="C2" s="12"/>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -4708,23 +4899,24 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:10">
+      <c r="G2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="11"/>
+        <v>80</v>
+      </c>
+      <c r="C3" s="12"/>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -4732,23 +4924,24 @@
       <c r="F3" s="1">
         <v>-1</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:10">
+      <c r="G3" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="11"/>
+        <v>83</v>
+      </c>
+      <c r="C4" s="12"/>
       <c r="D4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -4756,23 +4949,24 @@
       <c r="F4" s="1">
         <v>-2</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A5" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="G4" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:11">
+      <c r="A5" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="B5" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="12"/>
       <c r="D5" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -4780,23 +4974,24 @@
       <c r="F5" s="1">
         <v>-5</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-    </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A6" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="G5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+    </row>
+    <row r="6" ht="15.1" customHeight="1" spans="1:11">
+      <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="12"/>
       <c r="D6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -4804,22 +4999,23 @@
       <c r="F6" s="1">
         <v>-3</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A7" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="G6" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+    </row>
+    <row r="7" ht="15.1" customHeight="1" spans="1:10">
+      <c r="A7" s="12" t="s">
         <v>91</v>
       </c>
+      <c r="B7" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -4827,14 +5023,15 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="G7" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K7">
+  <autoFilter ref="A1:L7">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4846,23 +5043,23 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="9" width="16.3916666666667" style="4"/>
-    <col min="10" max="1025" width="9.10833333333333" style="4"/>
+    <col min="1" max="10" width="16.3916666666667" style="5"/>
+    <col min="11" max="1026" width="9.10833333333333" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.95" customHeight="1" spans="1:9">
+    <row r="1" ht="12.95" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4870,13 +5067,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -4885,122 +5082,125 @@
         <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>97</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>97</v>
+      <c r="A4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>97</v>
+      <c r="A5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>97</v>
+      <c r="A6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>97</v>
+      <c r="A7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>97</v>
+      <c r="A8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>97</v>
+      <c r="A9" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -5016,26 +5216,26 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="2" width="10.7166666666667" style="4"/>
-    <col min="3" max="3" width="10.7166666666667" style="5"/>
-    <col min="4" max="5" width="10.6" style="5"/>
-    <col min="6" max="11" width="8.78333333333333" style="5"/>
-    <col min="12" max="1025" width="8.78333333333333" style="4"/>
+    <col min="1" max="2" width="10.7166666666667" style="5"/>
+    <col min="3" max="3" width="10.7166666666667" style="6"/>
+    <col min="4" max="5" width="10.6" style="6"/>
+    <col min="6" max="12" width="8.78333333333333" style="6"/>
+    <col min="13" max="1026" width="8.78333333333333" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:11">
+    <row r="1" ht="15" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5043,19 +5243,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -5064,143 +5264,152 @@
         <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:9">
-      <c r="A2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="19">
+    <row r="2" ht="15" customHeight="1" spans="1:10">
+      <c r="A2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="20">
         <v>0.000148</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="20">
         <v>0.0121655250605964</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" ht="15" customHeight="1" spans="1:9">
-      <c r="A3" s="4" t="s">
+      <c r="G2" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="19">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" spans="1:10">
+      <c r="A3" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="20">
         <v>0.0002</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="20">
         <v>0.014142135623731</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="1:9">
-      <c r="A4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="19">
+      <c r="G3" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:10">
+      <c r="A4" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="20">
         <v>0.0005</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="20">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:9">
-      <c r="A5" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="G4" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="1:10">
+      <c r="A5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="20">
         <v>0.0005</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="20">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="1:9">
-      <c r="A6" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="19">
+      <c r="G5" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:10">
+      <c r="A6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="20">
         <v>0.001</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="20">
         <v>0.0316227766016838</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="19">
+      <c r="G6" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="1:10">
+      <c r="A7" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="20">
         <v>0.002</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="20">
         <v>0.0447213595499958</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="G7" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5212,22 +5421,22 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="4"/>
+    <col min="1" max="1026" width="8.78333333333333" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:8">
+    <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5235,10 +5444,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -5247,9 +5456,12 @@
         <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replacing type enumerations with ontology
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="989" activeTab="3"/>
+    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="989" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="212">
   <si>
     <t>Id</t>
   </si>
@@ -406,7 +406,7 @@
     <t>WCM:0000006 ! fluid compartment</t>
   </si>
   <si>
-    <t>WCM:0000009 ! 3d compartment</t>
+    <t>WCM:0000009 ! 3D compartment</t>
   </si>
   <si>
     <t>e</t>
@@ -415,7 +415,7 @@
     <t>g</t>
   </si>
   <si>
-    <t>normal</t>
+    <t>WCM:0000065 ! normal distribution</t>
   </si>
   <si>
     <t>l</t>
@@ -463,7 +463,7 @@
     <t>NaHCO</t>
   </si>
   <si>
-    <t>pseudo_species</t>
+    <t>WCM:0000019 ! pseudo-species</t>
   </si>
   <si>
     <t>specie_2</t>
@@ -670,9 +670,6 @@
     <t>forward</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>k_cat_1 * max( specie_1[e], specie_2[e] )</t>
   </si>
   <si>
@@ -772,7 +769,7 @@
     <t>k_cat_2</t>
   </si>
   <si>
-    <t>k_cat</t>
+    <t>WCM:0000026 ! k_cat</t>
   </si>
   <si>
     <t>molecule^-1 s^-1</t>
@@ -781,7 +778,7 @@
     <t>k_m_3</t>
   </si>
   <si>
-    <t>K_m</t>
+    <t>WCM:0000027 ! K_m</t>
   </si>
   <si>
     <t>k_cat_1</t>
@@ -2346,7 +2343,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2409,11 +2406,9 @@
       <c r="D2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>132</v>
@@ -2425,7 +2420,7 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>134</v>
@@ -2433,11 +2428,9 @@
       <c r="D3" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>132</v>
@@ -2449,7 +2442,7 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>137</v>
@@ -2457,11 +2450,9 @@
       <c r="D4" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>132</v>
@@ -2473,19 +2464,17 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>132</v>
@@ -2497,7 +2486,7 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>140</v>
@@ -2505,11 +2494,9 @@
       <c r="D6" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>132</v>
@@ -2560,10 +2547,10 @@
         <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2583,7 +2570,7 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>38</v>
@@ -2644,7 +2631,7 @@
         <v>96</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -2664,10 +2651,10 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>38</v>
@@ -2679,7 +2666,7 @@
         <v>63</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2718,13 +2705,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>106</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>96</v>
@@ -2747,13 +2734,13 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>168</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>100</v>
@@ -2768,19 +2755,19 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K2" s="14"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>171</v>
-      </c>
       <c r="C3" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>101</v>
@@ -2797,13 +2784,13 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>173</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>102</v>
@@ -2820,13 +2807,13 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>175</v>
-      </c>
       <c r="C5" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>103</v>
@@ -2855,7 +2842,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2877,10 +2864,10 @@
         <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>96</v>
@@ -2903,14 +2890,12 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>147</v>
-      </c>
+      <c r="C2" s="6"/>
       <c r="D2" s="6">
         <v>0.3</v>
       </c>
@@ -2919,32 +2904,32 @@
         <v>34</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="D3" s="8">
         <v>2000</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="D4" s="8">
         <v>0.001</v>
@@ -2956,24 +2941,24 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>181</v>
+        <v>184</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>181</v>
+        <v>185</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -2984,30 +2969,30 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>181</v>
+        <v>186</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>181</v>
+        <v>187</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3015,15 +3000,13 @@
         <v>64</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>1100</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3031,31 +3014,27 @@
         <v>68</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1">
         <v>1100</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="9">
         <v>6.02214075862e+23</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3154,10 +3133,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>96</v>
@@ -3166,10 +3145,10 @@
         <v>74</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>29</v>
@@ -3184,22 +3163,22 @@
         <v>33</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>18</v>
@@ -3256,10 +3235,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>96</v>
@@ -3268,7 +3247,7 @@
         <v>74</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>18</v>
@@ -3418,46 +3397,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -4582,12 +4561,12 @@
   <sheetPr/>
   <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:C3"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -4665,7 +4644,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:E3"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -4836,12 +4815,14 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1026" width="8.78333333333333" style="1"/>
+    <col min="1" max="6" width="8.78333333333333" style="1"/>
+    <col min="7" max="7" width="27.25" style="1" customWidth="1"/>
+    <col min="8" max="1026" width="8.78333333333333" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:12">
@@ -5218,12 +5199,12 @@
   <sheetPr/>
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
@@ -5280,7 +5261,7 @@
       <c r="C2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E2" s="20">
@@ -5303,7 +5284,7 @@
       <c r="C3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E3" s="20">
@@ -5326,7 +5307,7 @@
       <c r="C4" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="20">
@@ -5349,7 +5330,7 @@
       <c r="C5" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E5" s="20">
@@ -5372,7 +5353,7 @@
       <c r="C6" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E6" s="20">
@@ -5395,7 +5376,7 @@
       <c r="C7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E7" s="20">

</xml_diff>

<commit_message>
replacing enum types with ontology; renaming Submodel.algorithm to Submodel.framework
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="989" activeTab="7"/>
+    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="989" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -334,7 +334,7 @@
     <t>dimensionless</t>
   </si>
   <si>
-    <t>Algorithm</t>
+    <t>Framework</t>
   </si>
   <si>
     <t>Evidence</t>
@@ -349,7 +349,7 @@
     <t>Metabolism</t>
   </si>
   <si>
-    <t>WCM:0000013 ! dFBA</t>
+    <t>dynamic_flux_balance_analysis</t>
   </si>
   <si>
     <t>For testing</t>
@@ -361,7 +361,7 @@
     <t>RNA degradation</t>
   </si>
   <si>
-    <t>WCM:0000011 ! SSA</t>
+    <t>stochastic_simulation_algorithm</t>
   </si>
   <si>
     <t>Biological type</t>
@@ -400,13 +400,13 @@
     <t>Cell</t>
   </si>
   <si>
-    <t>WCM:0000003 ! cellular compartment</t>
-  </si>
-  <si>
-    <t>WCM:0000006 ! fluid compartment</t>
-  </si>
-  <si>
-    <t>WCM:0000009 ! 3D compartment</t>
+    <t>cellular_compartment</t>
+  </si>
+  <si>
+    <t>fluid_compartment</t>
+  </si>
+  <si>
+    <t>3D_compartment</t>
   </si>
   <si>
     <t>e</t>
@@ -415,7 +415,7 @@
     <t>g</t>
   </si>
   <si>
-    <t>WCM:0000065 ! normal distribution</t>
+    <t>normal_distribution</t>
   </si>
   <si>
     <t>l</t>
@@ -430,7 +430,7 @@
     <t>Extracellular space</t>
   </si>
   <si>
-    <t>WCM:0000004 ! extracellular compartment</t>
+    <t>extracellular_compartment</t>
   </si>
   <si>
     <t>density_e</t>
@@ -463,7 +463,7 @@
     <t>NaHCO</t>
   </si>
   <si>
-    <t>WCM:0000019 ! pseudo-species</t>
+    <t>pseudo_species</t>
   </si>
   <si>
     <t>specie_2</t>
@@ -769,7 +769,7 @@
     <t>k_cat_2</t>
   </si>
   <si>
-    <t>WCM:0000026 ! k_cat</t>
+    <t>k_cat</t>
   </si>
   <si>
     <t>molecule^-1 s^-1</t>
@@ -778,7 +778,7 @@
     <t>k_m_3</t>
   </si>
   <si>
-    <t>WCM:0000027 ! K_m</t>
+    <t>K_m</t>
   </si>
   <si>
     <t>k_cat_1</t>
@@ -871,11 +871,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -941,10 +941,25 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -957,7 +972,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -972,21 +1009,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1006,6 +1029,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1016,39 +1046,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1067,31 +1067,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1109,7 +1091,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1121,7 +1109,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1133,13 +1151,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1151,31 +1163,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1187,19 +1175,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1217,13 +1211,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1235,19 +1235,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1305,47 +1305,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1367,122 +1326,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1492,10 +1492,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2406,7 +2406,6 @@
       <c r="D2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>147</v>
       </c>
@@ -2428,7 +2427,6 @@
       <c r="D3" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>149</v>
       </c>
@@ -2450,7 +2448,6 @@
       <c r="D4" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
         <v>151</v>
       </c>
@@ -2472,7 +2469,6 @@
       <c r="D5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>154</v>
       </c>
@@ -2494,7 +2490,6 @@
       <c r="D6" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>156</v>
       </c>
@@ -2842,7 +2837,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3:C4"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2895,7 +2890,6 @@
       <c r="B2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="6"/>
       <c r="D2" s="6">
         <v>0.3</v>
       </c>
@@ -4561,12 +4555,12 @@
   <sheetPr/>
   <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -4644,7 +4638,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -4815,7 +4809,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
@@ -5199,7 +5193,7 @@
   <sheetPr/>
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>

</xml_diff>

<commit_message>
adding TOCs to fixtures
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,231 +5,308 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="989" firstSheet="7" activeTab="17"/>
+    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="989"/>
   </bookViews>
   <sheets>
-    <sheet name="Model" sheetId="1" r:id="rId1"/>
-    <sheet name="Taxon" sheetId="2" r:id="rId2"/>
-    <sheet name="Environment" sheetId="19" r:id="rId3"/>
-    <sheet name="Submodels" sheetId="3" r:id="rId4"/>
-    <sheet name="Compartments" sheetId="4" r:id="rId5"/>
-    <sheet name="Species types" sheetId="5" r:id="rId6"/>
-    <sheet name="Species" sheetId="6" r:id="rId7"/>
-    <sheet name="Initial species concentrations" sheetId="7" r:id="rId8"/>
-    <sheet name="Observables" sheetId="8" r:id="rId9"/>
-    <sheet name="Functions" sheetId="9" r:id="rId10"/>
-    <sheet name="Reactions" sheetId="10" r:id="rId11"/>
-    <sheet name="Rate laws" sheetId="11" r:id="rId12"/>
-    <sheet name="dFBA objectives" sheetId="12" r:id="rId13"/>
-    <sheet name="dFBA objective reactions" sheetId="13" r:id="rId14"/>
-    <sheet name="dFBA objective species" sheetId="14" r:id="rId15"/>
-    <sheet name="Parameters" sheetId="15" r:id="rId16"/>
-    <sheet name="Stop conditions" sheetId="16" r:id="rId17"/>
-    <sheet name="Evidence" sheetId="17" r:id="rId18"/>
-    <sheet name="Interpretations" sheetId="20" r:id="rId19"/>
-    <sheet name="References" sheetId="18" r:id="rId20"/>
-    <sheet name="Authors" sheetId="21" r:id="rId21"/>
-    <sheet name="Changes" sheetId="22" r:id="rId22"/>
+    <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
+    <sheet name="Model" sheetId="1" r:id="rId2"/>
+    <sheet name="Taxon" sheetId="2" r:id="rId3"/>
+    <sheet name="Environment" sheetId="19" r:id="rId4"/>
+    <sheet name="Submodels" sheetId="3" r:id="rId5"/>
+    <sheet name="Compartments" sheetId="4" r:id="rId6"/>
+    <sheet name="Species types" sheetId="5" r:id="rId7"/>
+    <sheet name="Species" sheetId="6" r:id="rId8"/>
+    <sheet name="Initial species concentrations" sheetId="7" r:id="rId9"/>
+    <sheet name="Observables" sheetId="8" r:id="rId10"/>
+    <sheet name="Functions" sheetId="9" r:id="rId11"/>
+    <sheet name="Reactions" sheetId="10" r:id="rId12"/>
+    <sheet name="Rate laws" sheetId="11" r:id="rId13"/>
+    <sheet name="dFBA objectives" sheetId="12" r:id="rId14"/>
+    <sheet name="dFBA objective reactions" sheetId="13" r:id="rId15"/>
+    <sheet name="dFBA objective species" sheetId="14" r:id="rId16"/>
+    <sheet name="Parameters" sheetId="15" r:id="rId17"/>
+    <sheet name="Stop conditions" sheetId="16" r:id="rId18"/>
+    <sheet name="Evidence" sheetId="17" r:id="rId19"/>
+    <sheet name="Interpretations" sheetId="20" r:id="rId20"/>
+    <sheet name="References" sheetId="18" r:id="rId21"/>
+    <sheet name="Authors" sheetId="21" r:id="rId22"/>
+    <sheet name="Changes" sheetId="22" r:id="rId23"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Species types'!$A$1:$L$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Parameters!$A$1:$F$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">References!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">Compartments!$A$2:$P$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="10">Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="15">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="19">References!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$1:$L$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">References!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4">Submodels!#REF!</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$P$4</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="245">
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Number of objects</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Taxon</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Submodels</t>
+  </si>
+  <si>
+    <t>Compartments</t>
+  </si>
+  <si>
+    <t>Species types</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Initial species concentrations</t>
+  </si>
+  <si>
+    <t>Observables</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Reactions</t>
+  </si>
+  <si>
+    <t>Rate laws</t>
+  </si>
+  <si>
+    <t>dFBA objectives</t>
+  </si>
+  <si>
+    <t>dFBA objective reactions</t>
+  </si>
+  <si>
+    <t>dFBA objective species</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Stop conditions</t>
+  </si>
+  <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>Interpretations</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
   <si>
     <t>Id</t>
   </si>
@@ -303,9 +380,6 @@
     <t>Rank not used</t>
   </si>
   <si>
-    <t>References</t>
-  </si>
-  <si>
     <t>env</t>
   </si>
   <si>
@@ -330,12 +404,6 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>Evidence</t>
-  </si>
-  <si>
-    <t>Interpretations</t>
-  </si>
-  <si>
     <t>submodel_1</t>
   </si>
   <si>
@@ -540,9 +608,6 @@
     <t>specie_6[c]</t>
   </si>
   <si>
-    <t>Species</t>
-  </si>
-  <si>
     <t>dist-init-conc-specie_1[e]</t>
   </si>
   <si>
@@ -792,12 +857,6 @@
     <t>Genotype</t>
   </si>
   <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>Taxon</t>
-  </si>
-  <si>
     <t>Variant</t>
   </si>
   <si>
@@ -820,9 +879,6 @@
   </si>
   <si>
     <t>Method</t>
-  </si>
-  <si>
-    <t>Authors</t>
   </si>
   <si>
     <t>Title</t>
@@ -917,14 +973,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -951,31 +1007,29 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -987,7 +1041,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1002,7 +1056,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1020,6 +1089,29 @@
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1045,8 +1137,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1059,47 +1174,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1114,13 +1190,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFCCCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,7 +1208,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,13 +1220,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,7 +1250,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,13 +1304,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,7 +1352,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1210,91 +1370,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1334,26 +1416,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -1362,16 +1424,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1401,156 +1463,176 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1610,16 +1692,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1627,6 +1709,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2015,114 +2105,321 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A8" sqref="$A8:$XFD10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1" max="3" width="15.7083333333333" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="27" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+    <row r="1" customHeight="1" spans="1:3">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="28" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A2" s="2" t="s">
+    <row r="2" customHeight="1" spans="1:3">
+      <c r="A2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:3">
+      <c r="A3" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:3">
+      <c r="A4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:3">
+      <c r="A5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:3">
+      <c r="A6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="7" customHeight="1" spans="1:3">
+      <c r="A7" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:3">
+      <c r="A8" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:3">
+      <c r="A9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:3">
+      <c r="A10" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="11" customHeight="1" spans="1:3">
+      <c r="A11" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+    <row r="12" customHeight="1" spans="1:3">
+      <c r="A12" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29">
+        <v>175</v>
       </c>
     </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A5" s="2" t="s">
+    <row r="13" customHeight="1" spans="1:3">
+      <c r="A13" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:3">
+      <c r="A14" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:3">
+      <c r="A15" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:3">
+      <c r="A16" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:3">
+      <c r="A17" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:3">
+      <c r="A18" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:3">
+      <c r="A19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
+    <row r="20" customHeight="1" spans="1:3">
+      <c r="A20" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
+    <row r="21" customHeight="1" spans="1:3">
+      <c r="A21" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29">
+        <v>21</v>
       </c>
     </row>
-    <row r="8" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
+    <row r="22" customHeight="1" spans="1:3">
+      <c r="A22" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" ht="15.1" customHeight="1" spans="1:1">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" ht="15.1" customHeight="1" spans="1:1">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
+    <row r="23" customHeight="1" spans="1:3">
+      <c r="A23" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0" objects="1" scenarios="1"/>
+  <autoFilter ref="A1:C23">
+    <extLst/>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://github.com/org/repo"/>
+    <hyperlink ref="A2" location="'Model'!A1" display="Model" tooltip="Click to view model"/>
+    <hyperlink ref="A3" location="'Taxon'!A1" display="Taxon" tooltip="Click to view taxon"/>
+    <hyperlink ref="A4" location="'Environment'!A1" display="Environment" tooltip="Click to view environment"/>
+    <hyperlink ref="A5" location="'Submodels'!A1" display="Submodels" tooltip="Click to view submodels"/>
+    <hyperlink ref="A6" location="'Compartments'!A1" display="Compartments" tooltip="Click to view compartments"/>
+    <hyperlink ref="A7" location="'Species types'!A1" display="Species types" tooltip="Click to view species types"/>
+    <hyperlink ref="A8" location="'Species'!A1" display="Species" tooltip="Click to view species"/>
+    <hyperlink ref="A9" location="'Initial species concentrations'!A1" display="Initial species concentrations" tooltip="Click to view initial species concentrations"/>
+    <hyperlink ref="A10" location="'Observables'!A1" display="Observables" tooltip="Click to view observables"/>
+    <hyperlink ref="A11" location="'Functions'!A1" display="Functions" tooltip="Click to view functions"/>
+    <hyperlink ref="A12" location="'Reactions'!A1" display="Reactions" tooltip="Click to view reactions"/>
+    <hyperlink ref="A13" location="'Rate laws'!A1" display="Rate laws" tooltip="Click to view rate laws"/>
+    <hyperlink ref="A14" location="'dFBA objectives'!A1" display="dFBA objectives" tooltip="Click to view dfba objectives"/>
+    <hyperlink ref="A15" location="'dFBA objective reactions'!A1" display="dFBA objective reactions" tooltip="Click to view dfba objective reactions"/>
+    <hyperlink ref="A16" location="'dFBA objective species'!A1" display="dFBA objective species" tooltip="Click to view dfba objective species"/>
+    <hyperlink ref="A17" location="'Parameters'!A1" display="Parameters" tooltip="Click to view parameters"/>
+    <hyperlink ref="A18" location="'Stop conditions'!A1" display="Stop conditions" tooltip="Click to view stop conditions"/>
+    <hyperlink ref="A19" location="'Evidence'!A1" display="Evidence" tooltip="Click to view evidence"/>
+    <hyperlink ref="A20" location="'Interpretations'!A1" display="Interpretations" tooltip="Click to view interpretations"/>
+    <hyperlink ref="A21" location="'References'!A1" display="References" tooltip="Click to view references"/>
+    <hyperlink ref="A22" location="'Authors'!A1" display="Authors" tooltip="Click to view authors"/>
+    <hyperlink ref="A23" location="'Changes'!A1" display="Changes" tooltip="Click to view changes"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1026" width="8.78333333333333" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.1" customHeight="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I3"/>
@@ -2147,53 +2444,53 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2206,7 +2503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:N6"/>
@@ -2237,7 +2534,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="20" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
@@ -2249,66 +2546,66 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:14">
       <c r="A3" s="7" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="E3" s="7">
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
@@ -2317,69 +2614,69 @@
         <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="N3" s="21"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:14">
       <c r="A4" s="7" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="N4" s="21"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="E6" s="7">
         <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2395,7 +2692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:L6"/>
@@ -2422,57 +2719,57 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2481,19 +2778,19 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2502,19 +2799,19 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2523,19 +2820,19 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2544,19 +2841,19 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2566,7 +2863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:L3"/>
@@ -2589,66 +2886,66 @@
   <sheetData>
     <row r="1" spans="4:5">
       <c r="D1" s="18" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="E1" s="18"/>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2664,7 +2961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:J2"/>
@@ -2685,54 +2982,54 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="14" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="12" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2742,7 +3039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K5"/>
@@ -2765,84 +3062,84 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="14" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="15" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="E2" s="16">
         <v>-3</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="15" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="K2" s="15"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="15" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="E3" s="16">
         <v>-4</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2850,22 +3147,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="15" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="E4" s="16">
         <v>1</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2873,22 +3170,22 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="15" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="E5" s="16">
         <v>2</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2898,7 +3195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K11"/>
@@ -2921,148 +3218,148 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="7" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="D2" s="7">
         <v>0.3</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="7" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="8" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="D3" s="9">
         <v>2000</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="7" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="8" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="D4" s="9">
         <v>0.001</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="7" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="7" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="7" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3071,12 +3368,12 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -3085,12 +3382,12 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -3099,7 +3396,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3112,7 +3409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I1"/>
@@ -3134,31 +3431,31 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3171,12 +3468,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AMS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -3192,11 +3489,11 @@
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="7:1033">
       <c r="G1" s="5" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5" t="s">
-        <v>187</v>
+        <v>5</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -3209,70 +3506,70 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:1033">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AMQ2" s="1"/>
       <c r="AMR2" s="1"/>
@@ -3292,7 +3589,117 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="A8" sqref="$A8:$XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" ht="15.1" customHeight="1" spans="1:1">
+      <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" ht="15.1" customHeight="1" spans="1:1">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="https://github.com/org/repo"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:L9"/>
@@ -3315,40 +3722,40 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>197</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="3:4">
@@ -3393,74 +3800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight" activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="1"/>
-    <col min="1026" max="16384" width="9" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8"/>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:1">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:R1"/>
@@ -3480,58 +3820,58 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:18">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3544,7 +3884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:M1"/>
@@ -3564,43 +3904,43 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:13">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3609,7 +3949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:Q1"/>
@@ -3629,55 +3969,55 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:17">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>197</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3687,6 +4027,73 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1025" width="8.78333333333333" style="1"/>
+    <col min="1026" max="16384" width="9" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" ht="15.1" customHeight="1" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AMD9"/>
@@ -3707,20 +4114,20 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1">
         <v>37</v>
@@ -3728,15 +4135,15 @@
     </row>
     <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1">
         <v>7.75</v>
@@ -3744,10 +4151,10 @@
     </row>
     <row r="6" s="26" customFormat="1" customHeight="1" spans="1:1018">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -4768,17 +5175,17 @@
     </row>
     <row r="7" customHeight="1" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4787,7 +5194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AMK3"/>
@@ -4808,54 +5215,54 @@
   <sheetData>
     <row r="1" s="8" customFormat="1" ht="15.1" customHeight="1" spans="1:1025">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AMK1" s="6"/>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4865,7 +5272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:XFD4"/>
@@ -4895,7 +5302,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="18" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -5920,55 +6327,55 @@
     </row>
     <row r="2" s="8" customFormat="1" ht="15.1" customHeight="1" spans="1:16384">
       <c r="A2" s="25" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AMO2"/>
       <c r="AMP2"/>
@@ -21329,28 +21736,28 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:16">
       <c r="A3" s="7" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="I3" s="10">
         <v>4.58e-17</v>
@@ -21359,39 +21766,39 @@
         <v>4.58e-18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="7" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:16">
       <c r="A4" s="7" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -21400,16 +21807,16 @@
         <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="7" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -21425,7 +21832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:L7"/>
@@ -21447,52 +21854,52 @@
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -21501,7 +21908,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
@@ -21510,14 +21917,14 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -21526,7 +21933,7 @@
         <v>-1</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -21535,14 +21942,14 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -21551,7 +21958,7 @@
         <v>-2</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -21560,14 +21967,14 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="13" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="1" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -21576,7 +21983,7 @@
         <v>-5</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
@@ -21585,14 +21992,14 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:11">
       <c r="A6" s="13" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="1" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -21601,7 +22008,7 @@
         <v>-3</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
@@ -21610,13 +22017,13 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="13" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -21625,7 +22032,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
@@ -21641,7 +22048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:J9"/>
@@ -21662,146 +22069,146 @@
   <sheetData>
     <row r="1" ht="12.95" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -21814,7 +22221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:L7"/>
@@ -21838,51 +22245,51 @@
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E2" s="23">
         <v>0.000148</v>
@@ -21891,7 +22298,7 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
@@ -21899,13 +22306,13 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:10">
       <c r="A3" s="6" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E3" s="23">
         <v>0.0002</v>
@@ -21914,7 +22321,7 @@
         <v>0.014142135623731</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
@@ -21922,13 +22329,13 @@
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:10">
       <c r="A4" s="6" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E4" s="23">
         <v>0.0005</v>
@@ -21937,7 +22344,7 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
@@ -21945,13 +22352,13 @@
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:10">
       <c r="A5" s="6" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E5" s="23">
         <v>0.0005</v>
@@ -21960,7 +22367,7 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
@@ -21968,13 +22375,13 @@
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:10">
       <c r="A6" s="6" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E6" s="23">
         <v>0.001</v>
@@ -21983,7 +22390,7 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
@@ -21991,13 +22398,13 @@
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:10">
       <c r="A7" s="6" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E7" s="23">
         <v>0.002</v>
@@ -22006,7 +22413,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
@@ -22017,61 +22424,4 @@
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1026" width="8.78333333333333" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adding more structure to data model
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="989" firstSheet="9" activeTab="19"/>
+    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="989" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -34,49 +34,49 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$R$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$T$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$1:$L$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$D$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$F$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">References!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$R$4</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="244">
   <si>
     <t>Table</t>
   </si>
@@ -452,328 +452,328 @@
     <t>Initial density</t>
   </si>
   <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>cellular_compartment</t>
+  </si>
+  <si>
+    <t>fluid_compartment</t>
+  </si>
+  <si>
+    <t>3D_compartment</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>normal_distribution</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>density_c</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
+  </si>
+  <si>
+    <t>Extracellular space</t>
+  </si>
+  <si>
+    <t>extracellular_compartment</t>
+  </si>
+  <si>
+    <t>density_e</t>
+  </si>
+  <si>
+    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1E9 cells/mL [Ref-0002].</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Empirical formula</t>
+  </si>
+  <si>
+    <t>Molecular weight</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>specie_1</t>
+  </si>
+  <si>
+    <t>specie_name_1</t>
+  </si>
+  <si>
+    <t>NaHCO</t>
+  </si>
+  <si>
+    <t>pseudo_species</t>
+  </si>
+  <si>
+    <t>specie_2</t>
+  </si>
+  <si>
+    <t>specie_name_2</t>
+  </si>
+  <si>
+    <t>N2O2P</t>
+  </si>
+  <si>
+    <t>specie_3</t>
+  </si>
+  <si>
+    <t>specie_name_3</t>
+  </si>
+  <si>
+    <t>N4O4P2</t>
+  </si>
+  <si>
+    <t>specie_4</t>
+  </si>
+  <si>
+    <t>specie_name_4</t>
+  </si>
+  <si>
+    <t>N10O10P5</t>
+  </si>
+  <si>
+    <t>specie_5</t>
+  </si>
+  <si>
+    <t>specie_name_5</t>
+  </si>
+  <si>
+    <t>N5O5</t>
+  </si>
+  <si>
+    <t>specie_6</t>
+  </si>
+  <si>
+    <t>specie_name_6</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>Species type</t>
+  </si>
+  <si>
+    <t>Compartment</t>
+  </si>
+  <si>
+    <t>specie_1[e]</t>
+  </si>
+  <si>
+    <t>molecule</t>
+  </si>
+  <si>
+    <t>specie_2[e]</t>
+  </si>
+  <si>
+    <t>specie_1[c]</t>
+  </si>
+  <si>
+    <t>specie_2[c]</t>
+  </si>
+  <si>
+    <t>specie_3[c]</t>
+  </si>
+  <si>
+    <t>specie_4[c]</t>
+  </si>
+  <si>
+    <t>specie_5[c]</t>
+  </si>
+  <si>
+    <t>specie_6[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_1[e]</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_2[e]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_2[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_4[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_5[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-specie_6[c]</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>volume_c</t>
+  </si>
+  <si>
+    <t>c / density_c</t>
+  </si>
+  <si>
+    <t>volume_e</t>
+  </si>
+  <si>
+    <t>e / density_e</t>
+  </si>
+  <si>
+    <t>Flux bounds</t>
+  </si>
+  <si>
+    <t>Submodel</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Reversible</t>
+  </si>
+  <si>
+    <t>Rate units</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>reaction_1</t>
+  </si>
+  <si>
+    <t>reaction_name_1</t>
+  </si>
+  <si>
+    <t>specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
+  </si>
+  <si>
+    <t>s^-1</t>
+  </si>
+  <si>
+    <t>M s^-1</t>
+  </si>
+  <si>
+    <t>reaction_2</t>
+  </si>
+  <si>
+    <t>reaction_name_2</t>
+  </si>
+  <si>
+    <t>[c]: (2) specie_2 ==&gt; specie_3</t>
+  </si>
+  <si>
+    <t>reaction_3</t>
+  </si>
+  <si>
+    <t>reaction_name_3</t>
+  </si>
+  <si>
+    <t>[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
+  </si>
+  <si>
+    <t>reaction_4</t>
+  </si>
+  <si>
+    <t>reaction_name_4</t>
+  </si>
+  <si>
+    <t>[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
+  </si>
+  <si>
+    <t>Reaction</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>reaction_1-forward</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>k_cat_1 * max( specie_1[e], specie_2[e] )</t>
+  </si>
+  <si>
+    <t>reaction_2-forward</t>
+  </si>
+  <si>
+    <t>k_cat_2 * specie_2[c]</t>
+  </si>
+  <si>
+    <t>reaction_3-forward</t>
+  </si>
+  <si>
+    <t>k_cat_3_for * specie_4[c] / (specie_4[c] + k_m_3 * Avogadro * volume_c)</t>
+  </si>
+  <si>
+    <t>reaction_3-backward</t>
+  </si>
+  <si>
+    <t>backward</t>
+  </si>
+  <si>
+    <t>k_cat_3_rev * (specie_5[c] + specie_6[c])</t>
+  </si>
+  <si>
+    <t>reaction_4-forward</t>
+  </si>
+  <si>
+    <t>k_cat_4 * specie_2[c]</t>
+  </si>
+  <si>
+    <t>Reaction rate units</t>
+  </si>
+  <si>
+    <t>Coefficient units</t>
+  </si>
+  <si>
+    <t>dfba-obj-submodel_1</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Cell size units</t>
+  </si>
+  <si>
+    <t>Metabolism_net_rxn</t>
+  </si>
+  <si>
+    <t>Metabolism net reaction</t>
+  </si>
+  <si>
+    <t>No comment</t>
+  </si>
+  <si>
+    <t>dFBA objective reaction</t>
+  </si>
+  <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>cellular_compartment</t>
-  </si>
-  <si>
-    <t>fluid_compartment</t>
-  </si>
-  <si>
-    <t>3D_compartment</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>normal_distribution</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>density_c</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
-  </si>
-  <si>
-    <t>Extracellular space</t>
-  </si>
-  <si>
-    <t>extracellular_compartment</t>
-  </si>
-  <si>
-    <t>density_e</t>
-  </si>
-  <si>
-    <t>Typical density of Mycoplasma pneumoniae cells in culture is 1E9 cells/mL [Ref-0002].</t>
-  </si>
-  <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>Empirical formula</t>
-  </si>
-  <si>
-    <t>Molecular weight</t>
-  </si>
-  <si>
-    <t>Charge</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>specie_1</t>
-  </si>
-  <si>
-    <t>specie_name_1</t>
-  </si>
-  <si>
-    <t>NaHCO</t>
-  </si>
-  <si>
-    <t>pseudo_species</t>
-  </si>
-  <si>
-    <t>specie_2</t>
-  </si>
-  <si>
-    <t>specie_name_2</t>
-  </si>
-  <si>
-    <t>N2O2P</t>
-  </si>
-  <si>
-    <t>specie_3</t>
-  </si>
-  <si>
-    <t>specie_name_3</t>
-  </si>
-  <si>
-    <t>N4O4P2</t>
-  </si>
-  <si>
-    <t>specie_4</t>
-  </si>
-  <si>
-    <t>specie_name_4</t>
-  </si>
-  <si>
-    <t>N10O10P5</t>
-  </si>
-  <si>
-    <t>specie_5</t>
-  </si>
-  <si>
-    <t>specie_name_5</t>
-  </si>
-  <si>
-    <t>N5O5</t>
-  </si>
-  <si>
-    <t>specie_6</t>
-  </si>
-  <si>
-    <t>specie_name_6</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>Species type</t>
-  </si>
-  <si>
-    <t>Compartment</t>
-  </si>
-  <si>
-    <t>specie_1[e]</t>
-  </si>
-  <si>
-    <t>molecule</t>
-  </si>
-  <si>
-    <t>specie_2[e]</t>
-  </si>
-  <si>
-    <t>specie_1[c]</t>
-  </si>
-  <si>
-    <t>specie_2[c]</t>
-  </si>
-  <si>
-    <t>specie_3[c]</t>
-  </si>
-  <si>
-    <t>specie_4[c]</t>
-  </si>
-  <si>
-    <t>specie_5[c]</t>
-  </si>
-  <si>
-    <t>specie_6[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_1[e]</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_2[e]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_2[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_4[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_5[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-specie_6[c]</t>
-  </si>
-  <si>
-    <t>Expression</t>
-  </si>
-  <si>
-    <t>volume_c</t>
-  </si>
-  <si>
-    <t>c / density_c</t>
-  </si>
-  <si>
-    <t>volume_e</t>
-  </si>
-  <si>
-    <t>e / density_e</t>
-  </si>
-  <si>
-    <t>Flux</t>
-  </si>
-  <si>
-    <t>Submodel</t>
-  </si>
-  <si>
-    <t>Participants</t>
-  </si>
-  <si>
-    <t>Reversible</t>
-  </si>
-  <si>
-    <t>Rate units</t>
-  </si>
-  <si>
-    <t>Minimum</t>
-  </si>
-  <si>
-    <t>Maximum</t>
-  </si>
-  <si>
-    <t>reaction_1</t>
-  </si>
-  <si>
-    <t>reaction_name_1</t>
-  </si>
-  <si>
-    <t>specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
-  </si>
-  <si>
-    <t>s^-1</t>
-  </si>
-  <si>
-    <t>M s^-1</t>
-  </si>
-  <si>
-    <t>reaction_2</t>
-  </si>
-  <si>
-    <t>reaction_name_2</t>
-  </si>
-  <si>
-    <t>[c]: (2) specie_2 ==&gt; specie_3</t>
-  </si>
-  <si>
-    <t>reaction_3</t>
-  </si>
-  <si>
-    <t>reaction_name_3</t>
-  </si>
-  <si>
-    <t>[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
-  </si>
-  <si>
-    <t>reaction_4</t>
-  </si>
-  <si>
-    <t>reaction_name_4</t>
-  </si>
-  <si>
-    <t>[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
-  </si>
-  <si>
-    <t>Reaction</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>reaction_1-forward</t>
-  </si>
-  <si>
-    <t>forward</t>
-  </si>
-  <si>
-    <t>k_cat_1 * max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t>reaction_2-forward</t>
-  </si>
-  <si>
-    <t>k_cat_2 * specie_2[c]</t>
-  </si>
-  <si>
-    <t>reaction_3-forward</t>
-  </si>
-  <si>
-    <t>k_cat_3_for * specie_4[c] / (specie_4[c] + k_m_3 * Avogadro * volume_c)</t>
-  </si>
-  <si>
-    <t>reaction_3-backward</t>
-  </si>
-  <si>
-    <t>backward</t>
-  </si>
-  <si>
-    <t>k_cat_3_rev * (specie_5[c] + specie_6[c])</t>
-  </si>
-  <si>
-    <t>reaction_4-forward</t>
-  </si>
-  <si>
-    <t>k_cat_4 * specie_2[c]</t>
-  </si>
-  <si>
-    <t>Reaction rate units</t>
-  </si>
-  <si>
-    <t>Coefficient units</t>
-  </si>
-  <si>
-    <t>dfba-obj-submodel_1</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Cell size units</t>
-  </si>
-  <si>
-    <t>Metabolism_net_rxn</t>
-  </si>
-  <si>
-    <t>Metabolism net reaction</t>
-  </si>
-  <si>
-    <t>No comment</t>
-  </si>
-  <si>
-    <t>dFBA objective reaction</t>
   </si>
   <si>
     <t>dfba-net-species-Metabolism_net_rxn-specie_1[c]</t>
@@ -970,12 +970,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
-    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="177" formatCode="0.000E+00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1024,26 +1024,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1053,13 +1046,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1075,45 +1067,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1128,7 +1083,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1136,15 +1091,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1159,7 +1113,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1186,7 +1186,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,13 +1216,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1222,19 +1342,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1246,127 +1360,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,6 +1386,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1421,29 +1454,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1465,160 +1478,147 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1676,29 +1676,29 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2378,7 +2378,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
@@ -2428,8 +2428,8 @@
     <col min="2" max="2" width="8.78333333333333" style="1"/>
     <col min="3" max="3" width="11" style="1" customWidth="1"/>
     <col min="4" max="1024" width="8.78333333333333" style="1"/>
-    <col min="1025" max="1026" width="8.78333333333333" style="23"/>
-    <col min="1027" max="16384" width="9" style="23"/>
+    <col min="1025" max="1026" width="8.78333333333333" style="22"/>
+    <col min="1027" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:9">
@@ -2440,7 +2440,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
@@ -2463,24 +2463,24 @@
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2498,12 +2498,12 @@
   <sheetPr/>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD2"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2523,11 +2523,11 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="G1" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
@@ -2542,22 +2542,22 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>71</v>
@@ -2580,22 +2580,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:14">
       <c r="A3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>145</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G3" s="8">
         <v>0</v>
@@ -2604,69 +2604,69 @@
         <v>1</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="N3" s="22"/>
+        <v>147</v>
+      </c>
+      <c r="N3" s="21"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:14">
       <c r="A4" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="N4" s="22"/>
+        <v>146</v>
+      </c>
+      <c r="N4" s="21"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>156</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>157</v>
+      <c r="D6" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="E6" s="8">
         <v>0</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2715,16 +2715,16 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>71</v>
@@ -2747,19 +2747,19 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2768,19 +2768,19 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2789,19 +2789,19 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:12">
       <c r="A4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2810,19 +2810,19 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:12">
       <c r="A5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2831,19 +2831,19 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2856,17 +2856,17 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1:L2"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="25.925" style="1"/>
     <col min="2" max="3" width="9.10833333333333" style="1"/>
@@ -2874,74 +2874,65 @@
     <col min="5" max="1028" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:5">
-      <c r="D1" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="19"/>
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:12">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    <row r="2" ht="15.1" customHeight="1" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -2978,13 +2969,13 @@
         <v>27</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>71</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
@@ -3004,22 +2995,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>178</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>54</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3058,13 +3049,13 @@
         <v>27</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>71</v>
@@ -3093,16 +3084,16 @@
         <v>182</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E2" s="17">
         <v>-3</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3120,16 +3111,16 @@
         <v>185</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="17">
         <v>-4</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -3143,16 +3134,16 @@
         <v>187</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -3166,16 +3157,16 @@
         <v>189</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E5" s="17">
         <v>2</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3214,10 +3205,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>190</v>
@@ -3253,7 +3244,7 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>193</v>
@@ -3288,7 +3279,7 @@
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
@@ -3316,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
@@ -3349,7 +3340,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3363,7 +3354,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -3427,7 +3418,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
@@ -3510,7 +3501,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>190</v>
@@ -3519,7 +3510,7 @@
         <v>71</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>4</v>
@@ -3710,7 +3701,7 @@
   <sheetPr/>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -3740,7 +3731,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>190</v>
@@ -3749,7 +3740,7 @@
         <v>71</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>27</v>
@@ -3856,7 +3847,7 @@
         <v>219</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>220</v>
@@ -3990,7 +3981,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>236</v>
@@ -4265,18 +4256,18 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD2"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="15" width="8.78333333333333" style="8"/>
-    <col min="16" max="17" width="8.875" style="8" customWidth="1"/>
-    <col min="18" max="1030" width="8.78333333333333" style="8"/>
-    <col min="1031" max="1033" width="8.78333333333333"/>
+    <col min="1" max="17" width="8.78333333333333" style="8"/>
+    <col min="18" max="19" width="8.875" style="8" customWidth="1"/>
+    <col min="20" max="1032" width="8.78333333333333" style="8"/>
+    <col min="1033" max="1035" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:1030">
+    <row r="1" ht="15" customHeight="1" spans="1:1032">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -4284,19 +4275,19 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="9"/>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
@@ -5311,9 +5302,11 @@
       <c r="AMN1" s="9"/>
       <c r="AMO1" s="9"/>
       <c r="AMP1" s="9"/>
+      <c r="AMQ1" s="9"/>
+      <c r="AMR1" s="9"/>
     </row>
     <row r="2" s="9" customFormat="1" ht="15.1" customHeight="1" spans="1:16384">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5350,28 +5343,32 @@
         <v>72</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AMQ2"/>
-      <c r="AMR2"/>
       <c r="AMS2"/>
       <c r="AMT2"/>
       <c r="AMU2"/>
@@ -20725,30 +20722,30 @@
       <c r="XFC2"/>
       <c r="XFD2"/>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:18">
+    <row r="3" ht="15.1" customHeight="1" spans="1:20">
       <c r="A3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="I3" s="11">
         <v>4.58e-17</v>
@@ -20757,45 +20754,51 @@
         <v>4.58e-18</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.775</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M3" s="1">
-        <v>7.75</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="8" t="s">
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:20">
+      <c r="A4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:18">
-      <c r="A4" s="8" t="s">
+      <c r="C4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -20804,31 +20807,37 @@
         <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.775</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="M4" s="1">
-        <v>7.75</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R4">
+  <autoFilter ref="A2:T4">
     <extLst/>
   </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="H1:K1"/>
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -20864,19 +20873,19 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>40</v>
@@ -20896,14 +20905,14 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -20911,24 +20920,24 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="G2" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -20936,24 +20945,24 @@
       <c r="F3" s="1">
         <v>-1</v>
       </c>
-      <c r="G3" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
+      <c r="G3" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -20961,24 +20970,24 @@
       <c r="F4" s="1">
         <v>-2</v>
       </c>
-      <c r="G4" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
+      <c r="G4" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>106</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
@@ -20986,24 +20995,24 @@
       <c r="F5" s="1">
         <v>-5</v>
       </c>
-      <c r="G5" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
+      <c r="G5" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:11">
       <c r="A6" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>108</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>109</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -21011,23 +21020,23 @@
       <c r="F6" s="1">
         <v>-3</v>
       </c>
-      <c r="G6" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
+      <c r="G6" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="D7" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -21035,12 +21044,12 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
+      <c r="G7" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L7">
@@ -21079,10 +21088,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>71</v>
@@ -21105,114 +21114,114 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -21287,141 +21296,141 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:10">
       <c r="A2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0.000148</v>
+      </c>
+      <c r="F2" s="23">
+        <v>0.0121655250605964</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="24">
-        <v>0.000148</v>
-      </c>
-      <c r="F2" s="24">
-        <v>0.0121655250605964</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:10">
       <c r="A3" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="24">
+        <v>80</v>
+      </c>
+      <c r="E3" s="23">
         <v>0.0002</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>0.014142135623731</v>
       </c>
-      <c r="G3" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="G3" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:10">
       <c r="A4" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="24">
+        <v>80</v>
+      </c>
+      <c r="E4" s="23">
         <v>0.0005</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G4" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="G4" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:10">
       <c r="A5" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="24">
+        <v>80</v>
+      </c>
+      <c r="E5" s="23">
         <v>0.0005</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>0.0223606797749979</v>
       </c>
-      <c r="G5" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
+      <c r="G5" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:10">
       <c r="A6" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="24">
+        <v>80</v>
+      </c>
+      <c r="E6" s="23">
         <v>0.001</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>0.0316227766016838</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
+      <c r="G6" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:10">
       <c r="A7" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="24">
+        <v>80</v>
+      </c>
+      <c r="E7" s="23">
         <v>0.002</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>0.0447213595499958</v>
       </c>
-      <c r="G7" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
+      <c r="G7" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
integrating BpForms with wc-lang
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="989" firstSheet="5" activeTab="11"/>
+    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="989" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -35,7 +35,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$1:$L$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$D$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$F$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">References!$A$1:$D$1</definedName>
@@ -77,43 +77,43 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$1:$L$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="246">
   <si>
     <t>Table</t>
   </si>
@@ -503,6 +503,15 @@
     <t>Structure</t>
   </si>
   <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Alphabet</t>
+  </si>
+  <si>
     <t>Empirical formula</t>
   </si>
   <si>
@@ -521,7 +530,7 @@
     <t>specie_name_1</t>
   </si>
   <si>
-    <t>NaHCO</t>
+    <t>Na</t>
   </si>
   <si>
     <t>pseudo_species</t>
@@ -533,7 +542,7 @@
     <t>specie_name_2</t>
   </si>
   <si>
-    <t>N2O2P</t>
+    <t>OH</t>
   </si>
   <si>
     <t>specie_3</t>
@@ -542,7 +551,7 @@
     <t>specie_name_3</t>
   </si>
   <si>
-    <t>N4O4P2</t>
+    <t>O2H2</t>
   </si>
   <si>
     <t>specie_4</t>
@@ -551,7 +560,7 @@
     <t>specie_name_4</t>
   </si>
   <si>
-    <t>N10O10P5</t>
+    <t>O5H5</t>
   </si>
   <si>
     <t>specie_5</t>
@@ -560,7 +569,7 @@
     <t>specie_name_5</t>
   </si>
   <si>
-    <t>N5O5</t>
+    <t>OH2</t>
   </si>
   <si>
     <t>specie_6</t>
@@ -569,7 +578,7 @@
     <t>specie_name_6</t>
   </si>
   <si>
-    <t>P5</t>
+    <t>O3H</t>
   </si>
   <si>
     <t>Species type</t>
@@ -771,9 +780,6 @@
   </si>
   <si>
     <t>dFBA objective reaction</t>
-  </si>
-  <si>
-    <t>Value</t>
   </si>
   <si>
     <t>dfba-net-species-Metabolism_net_rxn-specie_1[c]</t>
@@ -970,10 +976,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1024,9 +1030,28 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1040,22 +1065,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1075,15 +1097,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1091,37 +1121,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1136,7 +1136,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1150,16 +1157,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1186,25 +1192,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1216,7 +1216,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1234,49 +1234,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1288,31 +1270,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1330,6 +1294,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1342,7 +1312,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1354,19 +1366,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1389,39 +1395,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1437,6 +1410,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1448,15 +1430,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1478,6 +1451,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1486,139 +1483,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1682,23 +1688,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2378,7 +2384,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
@@ -2440,7 +2446,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
@@ -2463,10 +2469,10 @@
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>81</v>
@@ -2474,10 +2480,10 @@
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>81</v>
@@ -2499,11 +2505,11 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:I2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2524,7 +2530,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="20" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
@@ -2542,22 +2548,22 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>71</v>
@@ -2580,22 +2586,22 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:14">
       <c r="A3" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G3" s="8">
         <v>0</v>
@@ -2604,69 +2610,69 @@
         <v>1</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="N3" s="21"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:14">
       <c r="A4" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="N4" s="21"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="8" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E6" s="8">
         <v>0</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2715,16 +2721,16 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>71</v>
@@ -2747,19 +2753,19 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2768,19 +2774,19 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2789,19 +2795,19 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2810,19 +2816,19 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2831,19 +2837,19 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2882,19 +2888,19 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>40</v>
@@ -2914,22 +2920,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2969,13 +2975,13 @@
         <v>27</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>71</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
@@ -2995,22 +3001,22 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="13" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>54</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>81</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3049,13 +3055,13 @@
         <v>27</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>71</v>
@@ -3078,49 +3084,49 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="16" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E2" s="17">
         <v>-3</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="16" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="K2" s="16"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E3" s="17">
         <v>-4</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -3128,22 +3134,22 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -3151,22 +3157,22 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="16" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E5" s="17">
         <v>2</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3205,13 +3211,13 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>71</v>
@@ -3234,10 +3240,10 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D2" s="8">
         <v>0.3</v>
@@ -3247,95 +3253,95 @@
         <v>83</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D3" s="10">
         <v>2000</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="9" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D4" s="10">
         <v>0.001</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="8" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="8" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3349,7 +3355,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3363,12 +3369,12 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -3377,7 +3383,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3418,7 +3424,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
@@ -3470,7 +3476,7 @@
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="7:1035">
       <c r="G1" s="6" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
@@ -3482,11 +3488,11 @@
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="Q1" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="R1" s="5"/>
       <c r="S1" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="T1" s="5"/>
       <c r="AMS1" s="1"/>
@@ -3501,22 +3507,22 @@
         <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>50</v>
@@ -3528,19 +3534,19 @@
         <v>62</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>27</v>
@@ -3719,7 +3725,7 @@
   <sheetData>
     <row r="1" spans="7:8">
       <c r="G1" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H1" s="5"/>
     </row>
@@ -3731,16 +3737,16 @@
         <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>27</v>
@@ -3835,46 +3841,46 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>40</v>
@@ -3919,28 +3925,28 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -3981,28 +3987,28 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -4023,7 +4029,7 @@
         <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -4275,19 +4281,19 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
       <c r="L1" s="9"/>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
@@ -5306,7 +5312,7 @@
       <c r="AMR1" s="9"/>
     </row>
     <row r="2" s="9" customFormat="1" ht="15.1" customHeight="1" spans="1:16384">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -20848,213 +20854,228 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G7"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="6" width="8.78333333333333" style="1"/>
-    <col min="7" max="7" width="27.25" style="1" customWidth="1"/>
-    <col min="8" max="1026" width="8.78333333333333" style="1"/>
+    <col min="1" max="8" width="8.78333333333333" style="1"/>
+    <col min="9" max="9" width="27.25" style="1" customWidth="1"/>
+    <col min="10" max="1028" width="8.78333333333333" style="1"/>
+    <col min="1029" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:12">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="3:8">
+      <c r="C1" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" spans="1:14">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:11">
-      <c r="A2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="1">
+    <row r="3" ht="15.1" customHeight="1" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="1">
+        <v>22.98976928</v>
+      </c>
+      <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
+      <c r="I3" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:11">
+    <row r="4" ht="15.1" customHeight="1" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
+        <v>17.007</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="1">
+        <v>34.014</v>
+      </c>
+      <c r="H5" s="1">
         <v>-2</v>
       </c>
-      <c r="G4" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
+      <c r="I5" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
     </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:11">
-      <c r="A5" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1">
+    <row r="6" ht="15.1" customHeight="1" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="1">
+        <v>85.035</v>
+      </c>
+      <c r="H6" s="1">
         <v>-5</v>
       </c>
-      <c r="G5" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
+      <c r="I6" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
     </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:11">
-      <c r="A6" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>-3</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
+    <row r="7" ht="15.1" customHeight="1" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="1">
+        <v>18.015</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
     </row>
-    <row r="7" ht="15.1" customHeight="1" spans="1:10">
-      <c r="A7" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
+    <row r="8" ht="15.1" customHeight="1" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="1">
+        <v>49.005</v>
+      </c>
+      <c r="H8" s="1">
+        <v>-5</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L7">
+  <autoFilter ref="A2:N8">
     <extLst/>
   </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="C1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
@@ -21088,10 +21109,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>71</v>
@@ -21114,114 +21135,114 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -21296,10 +21317,10 @@
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:10">
       <c r="A2" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>80</v>
@@ -21311,7 +21332,7 @@
         <v>0.0121655250605964</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
@@ -21319,10 +21340,10 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:10">
       <c r="A3" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>80</v>
@@ -21334,7 +21355,7 @@
         <v>0.014142135623731</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
@@ -21342,10 +21363,10 @@
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:10">
       <c r="A4" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>80</v>
@@ -21357,7 +21378,7 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
@@ -21365,10 +21386,10 @@
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:10">
       <c r="A5" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>80</v>
@@ -21380,7 +21401,7 @@
         <v>0.0223606797749979</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
@@ -21388,10 +21409,10 @@
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:10">
       <c r="A6" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>80</v>
@@ -21403,7 +21424,7 @@
         <v>0.0316227766016838</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
@@ -21411,10 +21432,10 @@
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:10">
       <c r="A7" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>80</v>
@@ -21426,7 +21447,7 @@
         <v>0.0447213595499958</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>

</xml_diff>

<commit_message>
aligning provenance with SEPIO
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="989"/>
+    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="989" firstSheet="13" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -34,86 +34,86 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$M$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$D$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$F$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">References!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="247">
   <si>
     <t>Table</t>
   </si>
@@ -885,6 +885,9 @@
   </si>
   <si>
     <t>Process</t>
+  </si>
+  <si>
+    <t>Interpretations</t>
   </si>
   <si>
     <t>Date</t>
@@ -2103,7 +2106,7 @@
   <sheetPr/>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
@@ -2361,22 +2364,22 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F$1:F$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1026" width="8.78333333333333" style="7"/>
+    <col min="1" max="1025" width="8.78333333333333" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
+    <row r="1" ht="15.1" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2393,15 +2396,12 @@
         <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2418,27 +2418,27 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F$1:F$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.78333333333333" style="1"/>
     <col min="3" max="3" width="11" style="1" customWidth="1"/>
-    <col min="4" max="1024" width="8.78333333333333" style="1"/>
-    <col min="1025" max="1026" width="8.78333333333333" style="22"/>
-    <col min="1027" max="16384" width="9" style="22"/>
+    <col min="4" max="1023" width="8.78333333333333" style="1"/>
+    <col min="1024" max="1025" width="8.78333333333333" style="22"/>
+    <col min="1026" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:9">
+    <row r="1" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2455,15 +2455,12 @@
         <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2502,14 +2499,14 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K$1:K$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2518,11 +2515,11 @@
     <col min="2" max="2" width="13.3916666666667" style="8"/>
     <col min="3" max="3" width="10.3916666666667" style="8"/>
     <col min="4" max="4" width="49.4916666666667" style="8"/>
-    <col min="5" max="14" width="8.78333333333333" style="8"/>
-    <col min="15" max="1027" width="8.78333333333333" style="9"/>
+    <col min="5" max="13" width="8.78333333333333" style="8"/>
+    <col min="14" max="1026" width="8.78333333333333" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2538,9 +2535,8 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:14">
+    <row r="2" ht="15.1" customHeight="1" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -2572,19 +2568,16 @@
         <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:14">
+    <row r="3" ht="15.1" customHeight="1" spans="1:13">
       <c r="A3" s="8" t="s">
         <v>146</v>
       </c>
@@ -2612,9 +2605,9 @@
       <c r="I3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="N3" s="21"/>
+      <c r="M3" s="21"/>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:14">
+    <row r="4" ht="15.1" customHeight="1" spans="1:13">
       <c r="A4" s="8" t="s">
         <v>151</v>
       </c>
@@ -2633,7 +2626,7 @@
       <c r="F4" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="N4" s="21"/>
+      <c r="M4" s="21"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="8" t="s">
@@ -2691,14 +2684,14 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E2:E6"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I$1:I$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2709,11 +2702,11 @@
     <col min="4" max="4" width="8.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="4.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="60.375" style="1" customWidth="1"/>
-    <col min="7" max="1024" width="8.78333333333333" style="1"/>
-    <col min="1025" max="1026" width="8.78333333333333"/>
+    <col min="7" max="1023" width="8.78333333333333" style="1"/>
+    <col min="1024" max="1025" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:12">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2739,19 +2732,16 @@
         <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:12">
+    <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>162</v>
       </c>
@@ -2770,9 +2760,8 @@
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
-      <c r="L2"/>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:12">
+    <row r="3" ht="15.1" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>165</v>
       </c>
@@ -2791,9 +2780,8 @@
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
-      <c r="L3"/>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:12">
+    <row r="4" ht="15.1" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>167</v>
       </c>
@@ -2812,9 +2800,8 @@
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
-      <c r="L4"/>
     </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:12">
+    <row r="5" ht="15.1" customHeight="1" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>169</v>
       </c>
@@ -2833,7 +2820,6 @@
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
-      <c r="L5"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -2862,14 +2848,14 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I$1:I$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2877,10 +2863,10 @@
     <col min="1" max="1" width="25.925" style="1"/>
     <col min="2" max="3" width="9.10833333333333" style="1"/>
     <col min="4" max="4" width="11.3583333333333" style="1"/>
-    <col min="5" max="1028" width="9.10833333333333" style="1"/>
+    <col min="5" max="1027" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:12">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2906,15 +2892,12 @@
         <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2951,23 +2934,23 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G$1:G$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="10" width="8.78333333333333" style="13"/>
-    <col min="11" max="1026" width="8.78333333333333" style="14"/>
+    <col min="1" max="9" width="8.78333333333333" style="13"/>
+    <col min="10" max="1025" width="8.78333333333333" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:10">
+    <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="15" t="s">
         <v>25</v>
       </c>
@@ -2987,19 +2970,16 @@
         <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="H1" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="I1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:9">
+    <row r="2" ht="15.1" customHeight="1" spans="1:8">
       <c r="A2" s="13" t="s">
         <v>179</v>
       </c>
@@ -3015,7 +2995,7 @@
       <c r="E2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3029,25 +3009,25 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H$1:H$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="5" width="8.78333333333333" style="13"/>
     <col min="6" max="6" width="8.78333333333333" style="7"/>
-    <col min="7" max="11" width="8.78333333333333" style="13"/>
-    <col min="12" max="1026" width="8.78333333333333" style="14"/>
+    <col min="7" max="10" width="8.78333333333333" style="13"/>
+    <col min="11" max="1025" width="8.78333333333333" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="15" t="s">
         <v>25</v>
       </c>
@@ -3070,19 +3050,16 @@
         <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="I1" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="J1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:11">
+    <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="16" t="s">
         <v>183</v>
       </c>
@@ -3103,13 +3080,12 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="K2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:9">
+    <row r="3" ht="15.1" customHeight="1" spans="1:8">
       <c r="A3" s="16" t="s">
         <v>186</v>
       </c>
@@ -3130,9 +3106,8 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:9">
+    <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="16" t="s">
         <v>188</v>
       </c>
@@ -3153,7 +3128,6 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="16" t="s">
@@ -3185,25 +3159,25 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H$1:H$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="5" width="8.78333333333333" style="8"/>
     <col min="6" max="6" width="16.175" style="8"/>
-    <col min="7" max="11" width="8.78333333333333" style="8"/>
-    <col min="12" max="1026" width="8.78333333333333" style="9"/>
+    <col min="7" max="10" width="8.78333333333333" style="8"/>
+    <col min="11" max="1025" width="8.78333333333333" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -3226,19 +3200,16 @@
         <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:10">
+    <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="8" t="s">
         <v>193</v>
       </c>
@@ -3252,7 +3223,7 @@
       <c r="F2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3399,24 +3370,24 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F$1:F$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1023" width="8.78333333333333" style="1"/>
-    <col min="1024" max="1024" width="8.78333333333333" style="7"/>
-    <col min="1025" max="1026" width="8.78333333333333"/>
+    <col min="1" max="1022" width="8.78333333333333" style="1"/>
+    <col min="1023" max="1023" width="8.78333333333333" style="7"/>
+    <col min="1024" max="1025" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
+    <row r="1" ht="15.1" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -3433,15 +3404,12 @@
         <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3458,23 +3426,23 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMU2"/>
+  <dimension ref="A1:AMT2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="V1" sqref="V$1:V$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="2" width="13.3916666666667" style="1"/>
-    <col min="3" max="1032" width="9.10833333333333" style="1"/>
+    <col min="3" max="1031" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="7:1035">
+    <row r="1" ht="15" customHeight="1" spans="7:1034">
       <c r="G1" s="6" t="s">
         <v>208</v>
       </c>
@@ -3495,11 +3463,11 @@
         <v>210</v>
       </c>
       <c r="T1" s="5"/>
+      <c r="AMR1" s="1"/>
       <c r="AMS1" s="1"/>
       <c r="AMT1" s="1"/>
-      <c r="AMU1" s="1"/>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:1035">
+    <row r="2" ht="15.1" customHeight="1" spans="1:1034">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -3564,17 +3532,14 @@
         <v>40</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="AMR2" s="1"/>
       <c r="AMS2" s="1"/>
       <c r="AMT2" s="1"/>
-      <c r="AMU2" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3707,12 +3672,12 @@
   <sheetPr/>
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3758,7 +3723,7 @@
         <v>40</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>20</v>
+        <v>218</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>41</v>
@@ -3770,7 +3735,7 @@
         <v>23</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="3:4">
@@ -3828,7 +3793,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3844,46 +3809,46 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>40</v>
@@ -3928,28 +3893,28 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -3967,14 +3932,14 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -3982,7 +3947,7 @@
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:17">
+    <row r="1" customHeight="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -3993,46 +3958,43 @@
         <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -4180,23 +4142,23 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMK3"/>
+  <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E$1:E$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1023" width="8.78333333333333" style="8"/>
-    <col min="1024" max="1026" width="8.78333333333333" style="7"/>
+    <col min="1" max="1022" width="8.78333333333333" style="8"/>
+    <col min="1023" max="1025" width="8.78333333333333" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" ht="15.1" customHeight="1" spans="1:1025">
+    <row r="1" s="9" customFormat="1" ht="15.1" customHeight="1" spans="1:1024">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -4210,20 +4172,17 @@
         <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AMK1" s="7"/>
+      <c r="AMJ1" s="7"/>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:7">
+    <row r="2" ht="15.1" customHeight="1" spans="1:6">
       <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
@@ -4233,7 +4192,7 @@
       <c r="C2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4258,25 +4217,25 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD4"/>
+  <dimension ref="A1:XFC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:P4"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R$1:R$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="17" width="8.78333333333333" style="8"/>
-    <col min="18" max="19" width="8.875" style="8" customWidth="1"/>
-    <col min="20" max="1032" width="8.78333333333333" style="8"/>
-    <col min="1033" max="1035" width="8.78333333333333"/>
+    <col min="18" max="18" width="8.875" style="8" customWidth="1"/>
+    <col min="19" max="1031" width="8.78333333333333" style="8"/>
+    <col min="1032" max="1034" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:1032">
+    <row r="1" ht="15" customHeight="1" spans="1:1031">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -5312,9 +5271,8 @@
       <c r="AMO1" s="9"/>
       <c r="AMP1" s="9"/>
       <c r="AMQ1" s="9"/>
-      <c r="AMR1" s="9"/>
     </row>
-    <row r="2" s="9" customFormat="1" ht="15.1" customHeight="1" spans="1:16384">
+    <row r="2" s="9" customFormat="1" ht="15.1" customHeight="1" spans="1:16383">
       <c r="A2" s="26" t="s">
         <v>25</v>
       </c>
@@ -5367,17 +5325,15 @@
         <v>40</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="AMR2"/>
       <c r="AMS2"/>
       <c r="AMT2"/>
       <c r="AMU2"/>
@@ -20729,9 +20685,8 @@
       <c r="XFA2"/>
       <c r="XFB2"/>
       <c r="XFC2"/>
-      <c r="XFD2"/>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:20">
+    <row r="3" ht="15.1" customHeight="1" spans="1:19">
       <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
@@ -20782,12 +20737,11 @@
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:20">
+    <row r="4" ht="15.1" customHeight="1" spans="1:19">
       <c r="A4" s="8" t="s">
         <v>78</v>
       </c>
@@ -20835,13 +20789,12 @@
       </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T4">
+  <autoFilter ref="A2:S4">
     <extLst/>
   </autoFilter>
   <mergeCells count="2">
@@ -20857,22 +20810,22 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3:H8"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K$1:K$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="8" width="8.78333333333333" style="1"/>
     <col min="9" max="9" width="27.25" style="1" customWidth="1"/>
-    <col min="10" max="1028" width="8.78333333333333" style="1"/>
-    <col min="1029" max="16384" width="9" style="22"/>
+    <col min="10" max="1027" width="8.78333333333333" style="1"/>
+    <col min="1028" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:8">
@@ -20885,7 +20838,7 @@
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:14">
+    <row r="2" ht="15.1" customHeight="1" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -20917,19 +20870,16 @@
         <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:13">
+    <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -20951,9 +20901,8 @@
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:13">
+    <row r="4" ht="15.1" customHeight="1" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
@@ -20975,9 +20924,8 @@
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
     </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:13">
+    <row r="5" ht="15.1" customHeight="1" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>104</v>
       </c>
@@ -20999,9 +20947,8 @@
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
     </row>
-    <row r="6" ht="15.1" customHeight="1" spans="1:13">
+    <row r="6" ht="15.1" customHeight="1" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
@@ -21023,9 +20970,8 @@
       <c r="J6" s="25"/>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
     </row>
-    <row r="7" ht="15.1" customHeight="1" spans="1:13">
+    <row r="7" ht="15.1" customHeight="1" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>110</v>
       </c>
@@ -21047,9 +20993,8 @@
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
     </row>
-    <row r="8" ht="15.1" customHeight="1" spans="1:12">
+    <row r="8" ht="15.1" customHeight="1" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>113</v>
       </c>
@@ -21070,10 +21015,9 @@
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N8">
+  <autoFilter ref="A2:M8">
     <extLst/>
   </autoFilter>
   <mergeCells count="1">
@@ -21088,23 +21032,23 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G$1:G$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="10" width="16.3916666666667" style="7"/>
-    <col min="11" max="1026" width="9.10833333333333" style="7"/>
+    <col min="1" max="9" width="16.3916666666667" style="7"/>
+    <col min="10" max="1025" width="9.10833333333333" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.95" customHeight="1" spans="1:10">
+    <row r="1" ht="12.95" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -21124,15 +21068,12 @@
         <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -21261,14 +21202,14 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D2:D7"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I$1:I$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
@@ -21276,11 +21217,11 @@
     <col min="1" max="2" width="10.7166666666667" style="7"/>
     <col min="3" max="3" width="10.7166666666667" style="8"/>
     <col min="4" max="5" width="10.6" style="8"/>
-    <col min="6" max="12" width="8.78333333333333" style="8"/>
-    <col min="13" max="1026" width="8.78333333333333" style="7"/>
+    <col min="6" max="11" width="8.78333333333333" style="8"/>
+    <col min="12" max="1025" width="8.78333333333333" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:12">
+    <row r="1" ht="15" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -21306,19 +21247,16 @@
         <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:10">
+    <row r="2" ht="15" customHeight="1" spans="1:9">
       <c r="A2" s="7" t="s">
         <v>127</v>
       </c>
@@ -21339,9 +21277,8 @@
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:10">
+    <row r="3" ht="15" customHeight="1" spans="1:9">
       <c r="A3" s="7" t="s">
         <v>129</v>
       </c>
@@ -21362,9 +21299,8 @@
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:10">
+    <row r="4" ht="15" customHeight="1" spans="1:9">
       <c r="A4" s="7" t="s">
         <v>130</v>
       </c>
@@ -21385,9 +21321,8 @@
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:10">
+    <row r="5" ht="15" customHeight="1" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>131</v>
       </c>
@@ -21408,9 +21343,8 @@
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:10">
+    <row r="6" ht="15" customHeight="1" spans="1:9">
       <c r="A6" s="7" t="s">
         <v>132</v>
       </c>
@@ -21431,9 +21365,8 @@
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:10">
+    <row r="7" ht="15" customHeight="1" spans="1:9">
       <c r="A7" s="7" t="s">
         <v>133</v>
       </c>
@@ -21454,7 +21387,6 @@
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
cleaning up provenance data mdoel
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_model.xlsx
+++ b/tests/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="989" firstSheet="13" activeTab="19"/>
+    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="989" firstSheet="6" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -26,94 +26,95 @@
     <sheet name="dFBA objective species" sheetId="14" r:id="rId16"/>
     <sheet name="Parameters" sheetId="15" r:id="rId17"/>
     <sheet name="Stop conditions" sheetId="16" r:id="rId18"/>
-    <sheet name="Evidence" sheetId="17" r:id="rId19"/>
-    <sheet name="Conclusions" sheetId="20" r:id="rId20"/>
-    <sheet name="References" sheetId="18" r:id="rId21"/>
-    <sheet name="Authors" sheetId="21" r:id="rId22"/>
-    <sheet name="Changes" sheetId="22" r:id="rId23"/>
+    <sheet name="Observations" sheetId="17" r:id="rId19"/>
+    <sheet name="Observation sets" sheetId="24" r:id="rId20"/>
+    <sheet name="Conclusions" sheetId="20" r:id="rId21"/>
+    <sheet name="References" sheetId="18" r:id="rId22"/>
+    <sheet name="Authors" sheetId="21" r:id="rId23"/>
+    <sheet name="Changes" sheetId="22" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$M$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$D$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$F$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">References!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">References!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Submodels!#REF!</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$S$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$M$7</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="5">Compartments!$A$2:$T$4</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="6">'Species types'!$A$2:$N$7</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="11">Reactions!$A$2:$D$6</definedName>
@@ -188,50 +189,50 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="16">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="20">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="21">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="248">
   <si>
     <t>Table</t>
   </si>
@@ -293,108 +294,114 @@
     <t>Stop conditions</t>
   </si>
   <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Observation sets</t>
+  </si>
+  <si>
+    <t>Conclusions</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>ASP_test_2016_2</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ASP test model 2</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>https://github.com/org/repo</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>wc_lang version</t>
+  </si>
+  <si>
+    <t>Time units</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>Identifiers</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>taxon</t>
+  </si>
+  <si>
+    <t>Test model for TestExecutableModel</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>Rank not used</t>
+  </si>
+  <si>
+    <t>env</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Temperature units</t>
+  </si>
+  <si>
+    <t>degC</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
     <t>Evidence</t>
   </si>
   <si>
-    <t>Conclusions</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>Authors</t>
-  </si>
-  <si>
-    <t>Changes</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>ASP_test_2016_2</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>ASP test model 2</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>0.0.1</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>https://github.com/org/repo</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>master</t>
-  </si>
-  <si>
-    <t>Revision</t>
-  </si>
-  <si>
-    <t>hash</t>
-  </si>
-  <si>
-    <t>wc_lang version</t>
-  </si>
-  <si>
-    <t>Time units</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>Identifiers</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Created</t>
-  </si>
-  <si>
-    <t>Updated</t>
-  </si>
-  <si>
-    <t>taxon</t>
-  </si>
-  <si>
-    <t>Test model for TestExecutableModel</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>Rank not used</t>
-  </si>
-  <si>
-    <t>env</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Temperature units</t>
-  </si>
-  <si>
-    <t>degC</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>submodel_1</t>
   </si>
   <si>
@@ -885,9 +892,6 @@
   </si>
   <si>
     <t>Process</t>
-  </si>
-  <si>
-    <t>Interpretations</t>
   </si>
   <si>
     <t>Date</t>
@@ -2104,7 +2108,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2297,7 +2301,7 @@
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:3">
@@ -2306,7 +2310,7 @@
       </c>
       <c r="B21" s="29"/>
       <c r="C21" s="29">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:3">
@@ -2315,7 +2319,7 @@
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="29">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:3">
@@ -2327,9 +2331,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" customHeight="1" spans="1:3">
+      <c r="A24" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0" objects="1" scenarios="1"/>
-  <autoFilter ref="A1:C23">
+  <autoFilter ref="A1:C24">
     <extLst/>
   </autoFilter>
   <hyperlinks>
@@ -2350,11 +2363,12 @@
     <hyperlink ref="A16" location="'dFBA objective species'!A1" display="dFBA objective species" tooltip="Click to view dfba objective species"/>
     <hyperlink ref="A17" location="'Parameters'!A1" display="Parameters" tooltip="Click to view parameters"/>
     <hyperlink ref="A18" location="'Stop conditions'!A1" display="Stop conditions" tooltip="Click to view stop conditions"/>
-    <hyperlink ref="A19" location="'Evidence'!A1" display="Evidence" tooltip="Click to view evidence"/>
-    <hyperlink ref="A20" location="'Interpretations'!A1" display="Conclusions" tooltip="Click to view interpretations"/>
-    <hyperlink ref="A21" location="'References'!A1" display="References" tooltip="Click to view references"/>
-    <hyperlink ref="A22" location="'Authors'!A1" display="Authors" tooltip="Click to view authors"/>
-    <hyperlink ref="A23" location="'Changes'!A1" display="Changes" tooltip="Click to view changes"/>
+    <hyperlink ref="A21" location="'Interpretations'!A1" display="Conclusions" tooltip="Click to view interpretations"/>
+    <hyperlink ref="A22" location="'References'!A1" display="References" tooltip="Click to view references"/>
+    <hyperlink ref="A23" location="'Authors'!A1" display="Authors" tooltip="Click to view authors"/>
+    <hyperlink ref="A24" location="'Changes'!A1" display="Changes" tooltip="Click to view changes"/>
+    <hyperlink ref="A19" location="'Evidence'!A1" display="Observations" tooltip="Click to view evidence"/>
+    <hyperlink ref="A20" location="'Evidence'!A1" display="Observation sets" tooltip="Click to view evidence"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2364,45 +2378,48 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F$1:F$1048576"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="8.78333333333333" style="7"/>
+    <col min="1" max="1026" width="8.78333333333333" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:8">
+    <row r="1" ht="15.1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2418,72 +2435,75 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F$1:F$1048576"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.78333333333333" style="1"/>
     <col min="3" max="3" width="11" style="1" customWidth="1"/>
-    <col min="4" max="1023" width="8.78333333333333" style="1"/>
-    <col min="1024" max="1025" width="8.78333333333333" style="22"/>
-    <col min="1026" max="16384" width="9" style="22"/>
+    <col min="4" max="1024" width="8.78333333333333" style="1"/>
+    <col min="1025" max="1026" width="8.78333333333333" style="22"/>
+    <col min="1027" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:8">
+    <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2499,14 +2519,14 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K$1:K$1048576"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2515,11 +2535,11 @@
     <col min="2" max="2" width="13.3916666666667" style="8"/>
     <col min="3" max="3" width="10.3916666666667" style="8"/>
     <col min="4" max="4" width="49.4916666666667" style="8"/>
-    <col min="5" max="13" width="8.78333333333333" style="8"/>
-    <col min="14" max="1026" width="8.78333333333333" style="9"/>
+    <col min="5" max="14" width="8.78333333333333" style="8"/>
+    <col min="15" max="1027" width="8.78333333333333" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2527,7 +2547,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="20" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
@@ -2535,66 +2555,70 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:13">
+    <row r="2" ht="15.1" customHeight="1" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:13">
+    <row r="3" ht="15.1" customHeight="1" spans="1:14">
       <c r="A3" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G3" s="8">
         <v>0</v>
@@ -2603,69 +2627,69 @@
         <v>1</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="M3" s="21"/>
+        <v>152</v>
+      </c>
+      <c r="N3" s="21"/>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:13">
+    <row r="4" ht="15.1" customHeight="1" spans="1:14">
       <c r="A4" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="M4" s="21"/>
+        <v>151</v>
+      </c>
+      <c r="N4" s="21"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E6" s="8">
         <v>0</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2684,14 +2708,14 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I$1:I$1048576"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -2702,140 +2726,143 @@
     <col min="4" max="4" width="8.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="4.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="60.375" style="1" customWidth="1"/>
-    <col min="7" max="1023" width="8.78333333333333" style="1"/>
-    <col min="1024" max="1025" width="8.78333333333333"/>
+    <col min="7" max="1024" width="8.78333333333333" style="1"/>
+    <col min="1025" max="1026" width="8.78333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:11">
+    <row r="2" ht="15.1" customHeight="1" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I2"/>
+        <v>151</v>
+      </c>
       <c r="J2"/>
       <c r="K2"/>
+      <c r="L2"/>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:11">
+    <row r="3" ht="15.1" customHeight="1" spans="1:12">
       <c r="A3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
+      <c r="L3"/>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:11">
+    <row r="4" ht="15.1" customHeight="1" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4"/>
+        <v>151</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
+      <c r="L4"/>
     </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:11">
+    <row r="5" ht="15.1" customHeight="1" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I5"/>
+        <v>151</v>
+      </c>
       <c r="J5"/>
       <c r="K5"/>
+      <c r="L5"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2848,14 +2875,14 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I$1:I$1048576"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2863,62 +2890,65 @@
     <col min="1" max="1" width="25.925" style="1"/>
     <col min="2" max="3" width="9.10833333333333" style="1"/>
     <col min="4" max="4" width="11.3583333333333" style="1"/>
-    <col min="5" max="1027" width="9.10833333333333" style="1"/>
+    <col min="5" max="1028" width="9.10833333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:11">
+    <row r="1" ht="15.1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2934,69 +2964,72 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G$1:G$1048576"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="9" width="8.78333333333333" style="13"/>
-    <col min="10" max="1025" width="8.78333333333333" style="14"/>
+    <col min="1" max="10" width="8.78333333333333" style="13"/>
+    <col min="11" max="1026" width="8.78333333333333" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:9">
+    <row r="1" ht="15.1" customHeight="1" spans="1:10">
       <c r="A1" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>41</v>
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:8">
+    <row r="2" ht="15.1" customHeight="1" spans="1:9">
       <c r="A2" s="13" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>181</v>
+        <v>83</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3009,144 +3042,150 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H$1:H$1048576"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="5" width="8.78333333333333" style="13"/>
     <col min="6" max="6" width="8.78333333333333" style="7"/>
-    <col min="7" max="10" width="8.78333333333333" style="13"/>
-    <col min="11" max="1025" width="8.78333333333333" style="14"/>
+    <col min="7" max="11" width="8.78333333333333" style="13"/>
+    <col min="12" max="1026" width="8.78333333333333" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:10">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>41</v>
+        <v>55</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:10">
+    <row r="2" ht="15.1" customHeight="1" spans="1:11">
       <c r="A2" s="16" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E2" s="17">
         <v>-3</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="J2" s="16"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="K2" s="16"/>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:8">
+    <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E3" s="17">
         <v>-4</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:8">
+    <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
      